<commit_message>
Ileri Java Hafta 3
</commit_message>
<xml_diff>
--- a/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
+++ b/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>Adı</t>
   </si>
@@ -331,18 +331,6 @@
   </si>
   <si>
     <t>NOT</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>DEVAM DURUMU (%10)</t>
@@ -756,15 +744,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -778,15 +757,6 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -818,41 +788,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -870,6 +828,24 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -965,6 +941,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1000,196 +996,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1478,7 +1284,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK9" sqref="AK9"/>
+      <selection pane="bottomLeft" activeCell="AI28" sqref="AI28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1505,194 +1311,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="27"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="38"/>
     </row>
     <row r="2" spans="1:33" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41">
+      <c r="A2" s="35">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG2" s="28" t="s">
+      <c r="AG2" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="29" t="s">
         <v>91</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="31">
         <v>1</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="32">
         <v>2</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="32">
         <v>3</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="32">
         <v>4</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="32">
         <v>5</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="32">
         <v>6</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="32">
         <v>7</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="37">
+      <c r="L3" s="31">
         <v>1</v>
       </c>
-      <c r="M3" s="38">
+      <c r="M3" s="32">
         <v>2</v>
       </c>
-      <c r="N3" s="38">
+      <c r="N3" s="32">
         <v>3</v>
       </c>
-      <c r="O3" s="38">
+      <c r="O3" s="32">
         <v>4</v>
       </c>
-      <c r="P3" s="38">
+      <c r="P3" s="32">
         <v>5</v>
       </c>
-      <c r="Q3" s="38">
+      <c r="Q3" s="32">
         <v>6</v>
       </c>
-      <c r="R3" s="38">
+      <c r="R3" s="32">
         <v>7</v>
       </c>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="37">
+      <c r="T3" s="31">
         <v>1</v>
       </c>
-      <c r="U3" s="38">
+      <c r="U3" s="32">
         <v>2</v>
       </c>
-      <c r="V3" s="38">
+      <c r="V3" s="32">
         <v>3</v>
       </c>
-      <c r="W3" s="38">
+      <c r="W3" s="32">
         <v>4</v>
       </c>
-      <c r="X3" s="38">
+      <c r="X3" s="32">
         <v>5</v>
       </c>
-      <c r="Y3" s="39" t="s">
+      <c r="Y3" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="37">
+      <c r="Z3" s="31">
         <v>1</v>
       </c>
-      <c r="AA3" s="38">
+      <c r="AA3" s="32">
         <v>2</v>
       </c>
-      <c r="AB3" s="38">
+      <c r="AB3" s="32">
         <v>3</v>
       </c>
-      <c r="AC3" s="38">
+      <c r="AC3" s="32">
         <v>4</v>
       </c>
-      <c r="AD3" s="38">
+      <c r="AD3" s="32">
         <v>5</v>
       </c>
-      <c r="AE3" s="39" t="s">
+      <c r="AE3" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="AF3" s="37" t="s">
+      <c r="AF3" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="AG3" s="28" t="s">
+      <c r="AG3" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1701,7 +1507,7 @@
       <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>2</v>
       </c>
       <c r="E4" s="7">
@@ -1712,11 +1518,11 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="21">
-        <f>100*SUM(D4:J4)/(2*A$2)</f>
+      <c r="K4" s="18">
+        <f t="shared" ref="K4:K33" si="0">100*SUM(D4:J4)/(2*A$2)</f>
         <v>100</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="15">
         <v>100</v>
       </c>
       <c r="M4" s="6">
@@ -1727,36 +1533,36 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="21">
-        <f>SUM(L4:R4)/(A$2)</f>
+      <c r="S4" s="18">
+        <f t="shared" ref="S4:S33" si="1">SUM(L4:R4)/(A$2)</f>
         <v>100</v>
       </c>
-      <c r="T4" s="18"/>
+      <c r="T4" s="15"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="Y4" s="21">
-        <f>SUM(T4:X4)</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="18"/>
+      <c r="Y4" s="18">
+        <f t="shared" ref="Y4:Y33" si="2">SUM(T4:X4)</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="15"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
-      <c r="AE4" s="21">
-        <f>SUM(Z4:AD4)</f>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="30">
-        <f>K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
+      <c r="AE4" s="18">
+        <f t="shared" ref="AE4:AE33" si="3">SUM(Z4:AD4)</f>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="24">
+        <f t="shared" ref="AG4:AG33" si="4">K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="23" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1765,7 +1571,7 @@
       <c r="C5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>2</v>
       </c>
       <c r="E5" s="7">
@@ -1776,11 +1582,11 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="21">
-        <f>100*SUM(D5:J5)/(2*A$2)</f>
+      <c r="K5" s="18">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="15">
         <v>100</v>
       </c>
       <c r="M5" s="6">
@@ -1791,36 +1597,36 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="21">
-        <f>SUM(L5:R5)/(A$2)</f>
+      <c r="S5" s="18">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="T5" s="18"/>
+      <c r="T5" s="15"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
-      <c r="Y5" s="21">
-        <f>SUM(T5:X5)</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="18"/>
+      <c r="Y5" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="15"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
-      <c r="AE5" s="21">
-        <f>SUM(Z5:AD5)</f>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="30">
-        <f>K5*0.1+S5*0.2+Y5*0.2+AE5*0.2+AF5*0.3</f>
+      <c r="AE5" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="24">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1829,7 +1635,7 @@
       <c r="C6" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
       <c r="E6" s="7">
@@ -1840,11 +1646,11 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="21">
-        <f>100*SUM(D6:J6)/(2*A$2)</f>
+      <c r="K6" s="18">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="15">
         <v>100</v>
       </c>
       <c r="M6" s="6">
@@ -1855,36 +1661,36 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="21">
-        <f>SUM(L6:R6)/(A$2)</f>
+      <c r="S6" s="18">
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="T6" s="18"/>
+      <c r="T6" s="15"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
-      <c r="Y6" s="21">
-        <f>SUM(T6:X6)</f>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="18"/>
+      <c r="Y6" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="15"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
-      <c r="AE6" s="21">
-        <f>SUM(Z6:AD6)</f>
-        <v>0</v>
-      </c>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="30">
-        <f>K6*0.1+S6*0.2+Y6*0.2+AE6*0.2+AF6*0.3</f>
+      <c r="AE6" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="24">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1893,7 +1699,7 @@
       <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>2</v>
       </c>
       <c r="E7" s="7">
@@ -1904,11 +1710,11 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="21">
-        <f>100*SUM(D7:J7)/(2*A$2)</f>
+      <c r="K7" s="18">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="15">
         <v>100</v>
       </c>
       <c r="M7" s="6">
@@ -1919,36 +1725,36 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="S7" s="21">
-        <f>SUM(L7:R7)/(A$2)</f>
+      <c r="S7" s="18">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="T7" s="18"/>
+      <c r="T7" s="15"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
-      <c r="Y7" s="21">
-        <f>SUM(T7:X7)</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="18"/>
+      <c r="Y7" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="15"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
-      <c r="AE7" s="21">
-        <f>SUM(Z7:AD7)</f>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="30">
-        <f>K7*0.1+S7*0.2+Y7*0.2+AE7*0.2+AF7*0.3</f>
+      <c r="AE7" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="24">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1957,7 +1763,7 @@
       <c r="C8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>2</v>
       </c>
       <c r="E8" s="7">
@@ -1968,11 +1774,11 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="21">
-        <f>100*SUM(D8:J8)/(2*A$2)</f>
+      <c r="K8" s="18">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="15">
         <v>100</v>
       </c>
       <c r="M8" s="6">
@@ -1983,36 +1789,36 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="S8" s="21">
-        <f>SUM(L8:R8)/(A$2)</f>
+      <c r="S8" s="18">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="T8" s="18"/>
+      <c r="T8" s="15"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
-      <c r="Y8" s="21">
-        <f>SUM(T8:X8)</f>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="18"/>
+      <c r="Y8" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="15"/>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="21">
-        <f>SUM(Z8:AD8)</f>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="30">
-        <f>K8*0.1+S8*0.2+Y8*0.2+AE8*0.2+AF8*0.3</f>
+      <c r="AE8" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="24">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2021,7 +1827,7 @@
       <c r="C9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>1.7</v>
       </c>
       <c r="E9" s="7">
@@ -2032,11 +1838,11 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="21">
-        <f>100*SUM(D9:J9)/(2*A$2)</f>
+      <c r="K9" s="18">
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="15">
         <v>75</v>
       </c>
       <c r="M9" s="6">
@@ -2047,36 +1853,36 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
-      <c r="S9" s="21">
-        <f>SUM(L9:R9)/(A$2)</f>
+      <c r="S9" s="18">
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
-      <c r="T9" s="18"/>
+      <c r="T9" s="15"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
-      <c r="Y9" s="21">
-        <f>SUM(T9:X9)</f>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="18"/>
+      <c r="Y9" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="15"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
-      <c r="AE9" s="21">
-        <f>SUM(Z9:AD9)</f>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="30">
-        <f>K9*0.1+S9*0.2+Y9*0.2+AE9*0.2+AF9*0.3</f>
+      <c r="AE9" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="24">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2085,7 +1891,7 @@
       <c r="C10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>2</v>
       </c>
       <c r="E10" s="7">
@@ -2096,11 +1902,11 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="21">
-        <f>100*SUM(D10:J10)/(2*A$2)</f>
+      <c r="K10" s="18">
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="15">
         <v>100</v>
       </c>
       <c r="M10" s="6">
@@ -2111,36 +1917,36 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="21">
-        <f>SUM(L10:R10)/(A$2)</f>
+      <c r="S10" s="18">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="T10" s="18"/>
+      <c r="T10" s="15"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
-      <c r="Y10" s="21">
-        <f>SUM(T10:X10)</f>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="18"/>
+      <c r="Y10" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="15"/>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="21">
-        <f>SUM(Z10:AD10)</f>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="30">
-        <f>K10*0.1+S10*0.2+Y10*0.2+AE10*0.2+AF10*0.3</f>
+      <c r="AE10" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="24">
+        <f t="shared" si="4"/>
         <v>17.5</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2149,7 +1955,7 @@
       <c r="C11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>0</v>
       </c>
       <c r="E11" s="7">
@@ -2160,11 +1966,11 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="21">
-        <f>100*SUM(D11:J11)/(2*A$2)</f>
+      <c r="K11" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="15">
         <v>0</v>
       </c>
       <c r="M11" s="6">
@@ -2175,36 +1981,36 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="S11" s="21">
-        <f>SUM(L11:R11)/(A$2)</f>
+      <c r="S11" s="18">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="T11" s="18"/>
+      <c r="T11" s="15"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
-      <c r="Y11" s="21">
-        <f>SUM(T11:X11)</f>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="18"/>
+      <c r="Y11" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="15"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="21">
-        <f>SUM(Z11:AD11)</f>
-        <v>0</v>
-      </c>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="30">
-        <f>K11*0.1+S11*0.2+Y11*0.2+AE11*0.2+AF11*0.3</f>
+      <c r="AE11" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="24">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="23" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2213,7 +2019,7 @@
       <c r="C12" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>0</v>
       </c>
       <c r="E12" s="7">
@@ -2224,11 +2030,11 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="21">
-        <f>100*SUM(D12:J12)/(2*A$2)</f>
+      <c r="K12" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="15">
         <v>0</v>
       </c>
       <c r="M12" s="6">
@@ -2239,36 +2045,36 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="S12" s="21">
-        <f>SUM(L12:R12)/(A$2)</f>
+      <c r="S12" s="18">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="T12" s="18"/>
+      <c r="T12" s="15"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
-      <c r="Y12" s="21">
-        <f>SUM(T12:X12)</f>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="18"/>
+      <c r="Y12" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="15"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="21">
-        <f>SUM(Z12:AD12)</f>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="30">
-        <f>K12*0.1+S12*0.2+Y12*0.2+AE12*0.2+AF12*0.3</f>
+      <c r="AE12" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="24">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="23" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2277,7 +2083,7 @@
       <c r="C13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>0</v>
       </c>
       <c r="E13" s="7">
@@ -2288,11 +2094,11 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="21">
-        <f>100*SUM(D13:J13)/(2*A$2)</f>
+      <c r="K13" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="15">
         <v>0</v>
       </c>
       <c r="M13" s="6">
@@ -2303,36 +2109,36 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
-      <c r="S13" s="21">
-        <f>SUM(L13:R13)/(A$2)</f>
+      <c r="S13" s="18">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="T13" s="18"/>
+      <c r="T13" s="15"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
-      <c r="Y13" s="21">
-        <f>SUM(T13:X13)</f>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="18"/>
+      <c r="Y13" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="15"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
-      <c r="AE13" s="21">
-        <f>SUM(Z13:AD13)</f>
-        <v>0</v>
-      </c>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="30">
-        <f>K13*0.1+S13*0.2+Y13*0.2+AE13*0.2+AF13*0.3</f>
+      <c r="AE13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="24">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2341,7 +2147,7 @@
       <c r="C14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>0</v>
       </c>
       <c r="E14" s="7">
@@ -2352,11 +2158,11 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="21">
-        <f>100*SUM(D14:J14)/(2*A$2)</f>
+      <c r="K14" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="15">
         <v>0</v>
       </c>
       <c r="M14" s="6">
@@ -2367,36 +2173,36 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="21">
-        <f>SUM(L14:R14)/(A$2)</f>
+      <c r="S14" s="18">
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
-      <c r="T14" s="18"/>
+      <c r="T14" s="15"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
-      <c r="Y14" s="21">
-        <f>SUM(T14:X14)</f>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="18"/>
+      <c r="Y14" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="15"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
-      <c r="AE14" s="21">
-        <f>SUM(Z14:AD14)</f>
-        <v>0</v>
-      </c>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="30">
-        <f>K14*0.1+S14*0.2+Y14*0.2+AE14*0.2+AF14*0.3</f>
+      <c r="AE14" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="24">
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2405,7 +2211,7 @@
       <c r="C15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>0.5</v>
       </c>
       <c r="E15" s="7">
@@ -2416,11 +2222,11 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="21">
-        <f>100*SUM(D15:J15)/(2*A$2)</f>
+      <c r="K15" s="18">
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="15">
         <v>0</v>
       </c>
       <c r="M15" s="6">
@@ -2431,36 +2237,36 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="21">
-        <f>SUM(L15:R15)/(A$2)</f>
+      <c r="S15" s="18">
+        <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
-      <c r="T15" s="18"/>
+      <c r="T15" s="15"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
-      <c r="Y15" s="21">
-        <f>SUM(T15:X15)</f>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="18"/>
+      <c r="Y15" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="15"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
-      <c r="AE15" s="21">
-        <f>SUM(Z15:AD15)</f>
-        <v>0</v>
-      </c>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="30">
-        <f>K15*0.1+S15*0.2+Y15*0.2+AE15*0.2+AF15*0.3</f>
+      <c r="AE15" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="24">
+        <f t="shared" si="4"/>
         <v>12.25</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2469,7 +2275,7 @@
       <c r="C16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16" s="7">
@@ -2480,11 +2286,11 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="21">
-        <f>100*SUM(D16:J16)/(2*A$2)</f>
+      <c r="K16" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="15">
         <v>0</v>
       </c>
       <c r="M16" s="6">
@@ -2495,36 +2301,36 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="21">
-        <f>SUM(L16:R16)/(A$2)</f>
+      <c r="S16" s="18">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="T16" s="18"/>
+      <c r="T16" s="15"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
-      <c r="Y16" s="21">
-        <f>SUM(T16:X16)</f>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="18"/>
+      <c r="Y16" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="15"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
-      <c r="AE16" s="21">
-        <f>SUM(Z16:AD16)</f>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="30">
-        <f>K16*0.1+S16*0.2+Y16*0.2+AE16*0.2+AF16*0.3</f>
+      <c r="AE16" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="24">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2533,7 +2339,7 @@
       <c r="C17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>0</v>
       </c>
       <c r="E17" s="7">
@@ -2544,11 +2350,11 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="21">
-        <f>100*SUM(D17:J17)/(2*A$2)</f>
+      <c r="K17" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="15">
         <v>0</v>
       </c>
       <c r="M17" s="6">
@@ -2559,36 +2365,36 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="21">
-        <f>SUM(L17:R17)/(A$2)</f>
+      <c r="S17" s="18">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="T17" s="18"/>
+      <c r="T17" s="15"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
-      <c r="Y17" s="21">
-        <f>SUM(T17:X17)</f>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="18"/>
+      <c r="Y17" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="15"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
-      <c r="AE17" s="21">
-        <f>SUM(Z17:AD17)</f>
-        <v>0</v>
-      </c>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="30">
-        <f>K17*0.1+S17*0.2+Y17*0.2+AE17*0.2+AF17*0.3</f>
+      <c r="AE17" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="24">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2597,7 +2403,7 @@
       <c r="C18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>0</v>
       </c>
       <c r="E18" s="7">
@@ -2608,11 +2414,11 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="21">
-        <f>100*SUM(D18:J18)/(2*A$2)</f>
+      <c r="K18" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="15">
         <v>0</v>
       </c>
       <c r="M18" s="6">
@@ -2623,36 +2429,36 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="21">
-        <f>SUM(L18:R18)/(A$2)</f>
+      <c r="S18" s="18">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="T18" s="18"/>
+      <c r="T18" s="15"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
-      <c r="Y18" s="21">
-        <f>SUM(T18:X18)</f>
-        <v>0</v>
-      </c>
-      <c r="Z18" s="18"/>
+      <c r="Y18" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="15"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
-      <c r="AE18" s="21">
-        <f>SUM(Z18:AD18)</f>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="30">
-        <f>K18*0.1+S18*0.2+Y18*0.2+AE18*0.2+AF18*0.3</f>
+      <c r="AE18" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="24">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="23" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2661,7 +2467,7 @@
       <c r="C19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>0</v>
       </c>
       <c r="E19" s="7">
@@ -2672,11 +2478,11 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="21">
-        <f>100*SUM(D19:J19)/(2*A$2)</f>
+      <c r="K19" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="15">
         <v>0</v>
       </c>
       <c r="M19" s="6">
@@ -2687,36 +2493,36 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
-      <c r="S19" s="21">
-        <f>SUM(L19:R19)/(A$2)</f>
+      <c r="S19" s="18">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="T19" s="18"/>
+      <c r="T19" s="15"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
-      <c r="Y19" s="21">
-        <f>SUM(T19:X19)</f>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="18"/>
+      <c r="Y19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="15"/>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
-      <c r="AE19" s="21">
-        <f>SUM(Z19:AD19)</f>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="30">
-        <f>K19*0.1+S19*0.2+Y19*0.2+AE19*0.2+AF19*0.3</f>
+      <c r="AE19" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="24">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2725,7 +2531,7 @@
       <c r="C20" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>0</v>
       </c>
       <c r="E20" s="7">
@@ -2736,11 +2542,11 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="21">
-        <f>100*SUM(D20:J20)/(2*A$2)</f>
+      <c r="K20" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="15">
         <v>0</v>
       </c>
       <c r="M20" s="6">
@@ -2751,36 +2557,36 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="21">
-        <f>SUM(L20:R20)/(A$2)</f>
+      <c r="S20" s="18">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="T20" s="18"/>
+      <c r="T20" s="15"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
-      <c r="Y20" s="21">
-        <f>SUM(T20:X20)</f>
-        <v>0</v>
-      </c>
-      <c r="Z20" s="18"/>
+      <c r="Y20" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="15"/>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
-      <c r="AE20" s="21">
-        <f>SUM(Z20:AD20)</f>
-        <v>0</v>
-      </c>
-      <c r="AF20" s="18"/>
-      <c r="AG20" s="30">
-        <f>K20*0.1+S20*0.2+Y20*0.2+AE20*0.2+AF20*0.3</f>
+      <c r="AE20" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="24">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -2789,7 +2595,7 @@
       <c r="C21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>0</v>
       </c>
       <c r="E21" s="7">
@@ -2800,11 +2606,11 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="21">
-        <f>100*SUM(D21:J21)/(2*A$2)</f>
+      <c r="K21" s="18">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="15">
         <v>0</v>
       </c>
       <c r="M21" s="6">
@@ -2815,36 +2621,36 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
-      <c r="S21" s="21">
-        <f>SUM(L21:R21)/(A$2)</f>
+      <c r="S21" s="18">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="T21" s="18"/>
+      <c r="T21" s="15"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
-      <c r="Y21" s="21">
-        <f>SUM(T21:X21)</f>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="18"/>
+      <c r="Y21" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="15"/>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
-      <c r="AE21" s="21">
-        <f>SUM(Z21:AD21)</f>
-        <v>0</v>
-      </c>
-      <c r="AF21" s="18"/>
-      <c r="AG21" s="30">
-        <f>K21*0.1+S21*0.2+Y21*0.2+AE21*0.2+AF21*0.3</f>
+      <c r="AE21" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="24">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2853,7 +2659,7 @@
       <c r="C22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="12">
         <v>0</v>
       </c>
       <c r="E22" s="7">
@@ -2864,11 +2670,11 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
-      <c r="K22" s="21">
-        <f>100*SUM(D22:J22)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
+      <c r="K22" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
         <v>0</v>
       </c>
       <c r="M22" s="6">
@@ -2879,36 +2685,36 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
-      <c r="S22" s="21">
-        <f>SUM(L22:R22)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="18"/>
+      <c r="S22" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="15"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
-      <c r="Y22" s="21">
-        <f>SUM(T22:X22)</f>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="18"/>
+      <c r="Y22" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="15"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
-      <c r="AE22" s="21">
-        <f>SUM(Z22:AD22)</f>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="18"/>
-      <c r="AG22" s="30">
-        <f>K22*0.1+S22*0.2+Y22*0.2+AE22*0.2+AF22*0.3</f>
+      <c r="AE22" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2917,7 +2723,7 @@
       <c r="C23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>0</v>
       </c>
       <c r="E23" s="7">
@@ -2928,11 +2734,11 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="21">
-        <f>100*SUM(D23:J23)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
+      <c r="K23" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
         <v>0</v>
       </c>
       <c r="M23" s="6">
@@ -2943,36 +2749,36 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
-      <c r="S23" s="21">
-        <f>SUM(L23:R23)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T23" s="18"/>
+      <c r="S23" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="15"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
-      <c r="Y23" s="21">
-        <f>SUM(T23:X23)</f>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="18"/>
+      <c r="Y23" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="15"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
-      <c r="AE23" s="21">
-        <f>SUM(Z23:AD23)</f>
-        <v>0</v>
-      </c>
-      <c r="AF23" s="18"/>
-      <c r="AG23" s="30">
-        <f>K23*0.1+S23*0.2+Y23*0.2+AE23*0.2+AF23*0.3</f>
+      <c r="AE23" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2981,7 +2787,7 @@
       <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="12">
         <v>0</v>
       </c>
       <c r="E24" s="7">
@@ -2992,11 +2798,11 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="21">
-        <f>100*SUM(D24:J24)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="18">
+      <c r="K24" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
         <v>0</v>
       </c>
       <c r="M24" s="6">
@@ -3007,36 +2813,36 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
-      <c r="S24" s="21">
-        <f>SUM(L24:R24)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T24" s="18"/>
+      <c r="S24" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="15"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
-      <c r="Y24" s="21">
-        <f>SUM(T24:X24)</f>
-        <v>0</v>
-      </c>
-      <c r="Z24" s="18"/>
+      <c r="Y24" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="15"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
-      <c r="AE24" s="21">
-        <f>SUM(Z24:AD24)</f>
-        <v>0</v>
-      </c>
-      <c r="AF24" s="18"/>
-      <c r="AG24" s="30">
-        <f>K24*0.1+S24*0.2+Y24*0.2+AE24*0.2+AF24*0.3</f>
+      <c r="AE24" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -3045,7 +2851,7 @@
       <c r="C25" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="12">
         <v>0</v>
       </c>
       <c r="E25" s="7">
@@ -3056,11 +2862,11 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="21">
-        <f>100*SUM(D25:J25)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
+      <c r="K25" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="15">
         <v>0</v>
       </c>
       <c r="M25" s="6">
@@ -3071,36 +2877,36 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
-      <c r="S25" s="21">
-        <f>SUM(L25:R25)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T25" s="18"/>
+      <c r="S25" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="15"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
-      <c r="Y25" s="21">
-        <f>SUM(T25:X25)</f>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="18"/>
+      <c r="Y25" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="15"/>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
-      <c r="AE25" s="21">
-        <f>SUM(Z25:AD25)</f>
-        <v>0</v>
-      </c>
-      <c r="AF25" s="18"/>
-      <c r="AG25" s="30">
-        <f>K25*0.1+S25*0.2+Y25*0.2+AE25*0.2+AF25*0.3</f>
+      <c r="AE25" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -3109,7 +2915,7 @@
       <c r="C26" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="12">
         <v>0</v>
       </c>
       <c r="E26" s="7">
@@ -3120,11 +2926,11 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="21">
-        <f>100*SUM(D26:J26)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
+      <c r="K26" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
         <v>0</v>
       </c>
       <c r="M26" s="6">
@@ -3135,36 +2941,36 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="21">
-        <f>SUM(L26:R26)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T26" s="18"/>
+      <c r="S26" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="15"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
-      <c r="Y26" s="21">
-        <f>SUM(T26:X26)</f>
-        <v>0</v>
-      </c>
-      <c r="Z26" s="18"/>
+      <c r="Y26" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="15"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
-      <c r="AE26" s="21">
-        <f>SUM(Z26:AD26)</f>
-        <v>0</v>
-      </c>
-      <c r="AF26" s="18"/>
-      <c r="AG26" s="30">
-        <f>K26*0.1+S26*0.2+Y26*0.2+AE26*0.2+AF26*0.3</f>
+      <c r="AE26" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -3173,7 +2979,7 @@
       <c r="C27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="12">
         <v>0</v>
       </c>
       <c r="E27" s="7">
@@ -3184,11 +2990,11 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
-      <c r="K27" s="21">
-        <f>100*SUM(D27:J27)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
+      <c r="K27" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="15">
         <v>0</v>
       </c>
       <c r="M27" s="6">
@@ -3199,36 +3005,36 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
-      <c r="S27" s="21">
-        <f>SUM(L27:R27)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T27" s="18"/>
+      <c r="S27" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="15"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
-      <c r="Y27" s="21">
-        <f>SUM(T27:X27)</f>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="18"/>
+      <c r="Y27" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="15"/>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
-      <c r="AE27" s="21">
-        <f>SUM(Z27:AD27)</f>
-        <v>0</v>
-      </c>
-      <c r="AF27" s="18"/>
-      <c r="AG27" s="30">
-        <f>K27*0.1+S27*0.2+Y27*0.2+AE27*0.2+AF27*0.3</f>
+      <c r="AE27" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -3237,7 +3043,7 @@
       <c r="C28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="12">
         <v>0</v>
       </c>
       <c r="E28" s="7">
@@ -3248,11 +3054,11 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="21">
-        <f>100*SUM(D28:J28)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="18">
+      <c r="K28" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
         <v>0</v>
       </c>
       <c r="M28" s="6">
@@ -3263,36 +3069,36 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
-      <c r="S28" s="21">
-        <f>SUM(L28:R28)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T28" s="18"/>
+      <c r="S28" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="15"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
-      <c r="Y28" s="21">
-        <f>SUM(T28:X28)</f>
-        <v>0</v>
-      </c>
-      <c r="Z28" s="18"/>
+      <c r="Y28" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="15"/>
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
-      <c r="AE28" s="21">
-        <f>SUM(Z28:AD28)</f>
-        <v>0</v>
-      </c>
-      <c r="AF28" s="18"/>
-      <c r="AG28" s="30">
-        <f>K28*0.1+S28*0.2+Y28*0.2+AE28*0.2+AF28*0.3</f>
+      <c r="AE28" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3301,7 +3107,7 @@
       <c r="C29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="12">
         <v>0</v>
       </c>
       <c r="E29" s="7">
@@ -3312,11 +3118,11 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
-      <c r="K29" s="21">
-        <f>100*SUM(D29:J29)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="18">
+      <c r="K29" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
         <v>0</v>
       </c>
       <c r="M29" s="6">
@@ -3327,36 +3133,36 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
-      <c r="S29" s="21">
-        <f>SUM(L29:R29)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T29" s="18"/>
+      <c r="S29" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="15"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
-      <c r="Y29" s="21">
-        <f>SUM(T29:X29)</f>
-        <v>0</v>
-      </c>
-      <c r="Z29" s="18"/>
+      <c r="Y29" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="15"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
-      <c r="AE29" s="21">
-        <f>SUM(Z29:AD29)</f>
-        <v>0</v>
-      </c>
-      <c r="AF29" s="18"/>
-      <c r="AG29" s="30">
-        <f>K29*0.1+S29*0.2+Y29*0.2+AE29*0.2+AF29*0.3</f>
+      <c r="AE29" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="15"/>
+      <c r="AG29" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -3365,7 +3171,7 @@
       <c r="C30" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="12">
         <v>0</v>
       </c>
       <c r="E30" s="7">
@@ -3376,11 +3182,11 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="21">
-        <f>100*SUM(D30:J30)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="18">
+      <c r="K30" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
         <v>0</v>
       </c>
       <c r="M30" s="6">
@@ -3391,36 +3197,36 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="S30" s="21">
-        <f>SUM(L30:R30)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T30" s="18"/>
+      <c r="S30" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="15"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
-      <c r="Y30" s="21">
-        <f>SUM(T30:X30)</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="18"/>
+      <c r="Y30" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="15"/>
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
-      <c r="AE30" s="21">
-        <f>SUM(Z30:AD30)</f>
-        <v>0</v>
-      </c>
-      <c r="AF30" s="18"/>
-      <c r="AG30" s="30">
-        <f>K30*0.1+S30*0.2+Y30*0.2+AE30*0.2+AF30*0.3</f>
+      <c r="AE30" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -3429,7 +3235,7 @@
       <c r="C31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="12">
         <v>0</v>
       </c>
       <c r="E31" s="7">
@@ -3440,11 +3246,11 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="21">
-        <f>100*SUM(D31:J31)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="18">
+      <c r="K31" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
         <v>0</v>
       </c>
       <c r="M31" s="6">
@@ -3455,36 +3261,36 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
-      <c r="S31" s="21">
-        <f>SUM(L31:R31)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="18"/>
+      <c r="S31" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="15"/>
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
       <c r="W31" s="6"/>
       <c r="X31" s="6"/>
-      <c r="Y31" s="21">
-        <f>SUM(T31:X31)</f>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="18"/>
+      <c r="Y31" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="15"/>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
-      <c r="AE31" s="21">
-        <f>SUM(Z31:AD31)</f>
-        <v>0</v>
-      </c>
-      <c r="AF31" s="18"/>
-      <c r="AG31" s="30">
-        <f>K31*0.1+S31*0.2+Y31*0.2+AE31*0.2+AF31*0.3</f>
+      <c r="AE31" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF31" s="15"/>
+      <c r="AG31" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="23" t="s">
         <v>76</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -3493,7 +3299,7 @@
       <c r="C32" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="12">
         <v>0</v>
       </c>
       <c r="E32" s="7">
@@ -3504,11 +3310,11 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-      <c r="K32" s="21">
-        <f>100*SUM(D32:J32)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="18">
+      <c r="K32" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="15">
         <v>0</v>
       </c>
       <c r="M32" s="6">
@@ -3519,95 +3325,95 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
-      <c r="S32" s="21">
-        <f>SUM(L32:R32)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T32" s="18"/>
+      <c r="S32" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="15"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
-      <c r="Y32" s="21">
-        <f>SUM(T32:X32)</f>
-        <v>0</v>
-      </c>
-      <c r="Z32" s="18"/>
+      <c r="Y32" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z32" s="15"/>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
-      <c r="AE32" s="21">
-        <f>SUM(Z32:AD32)</f>
-        <v>0</v>
-      </c>
-      <c r="AF32" s="18"/>
-      <c r="AG32" s="30">
-        <f>K32*0.1+S32*0.2+Y32*0.2+AE32*0.2+AF32*0.3</f>
+      <c r="AE32" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF32" s="15"/>
+      <c r="AG32" s="24">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:33" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="16">
-        <v>0</v>
-      </c>
-      <c r="E33" s="17">
-        <v>0</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="21">
-        <f>100*SUM(D33:J33)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="18">
+      <c r="D33" s="13">
+        <v>0</v>
+      </c>
+      <c r="E33" s="14">
+        <v>0</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="15">
         <v>0</v>
       </c>
       <c r="M33" s="6">
         <v>0</v>
       </c>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="21">
-        <f>SUM(L33:R33)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T33" s="19"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
-      <c r="Y33" s="23">
-        <f>SUM(T33:X33)</f>
-        <v>0</v>
-      </c>
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
-      <c r="AD33" s="20"/>
-      <c r="AE33" s="21">
-        <f>SUM(Z33:AD33)</f>
-        <v>0</v>
-      </c>
-      <c r="AF33" s="19"/>
-      <c r="AG33" s="34">
-        <f>K33*0.1+S33*0.2+Y33*0.2+AE33*0.2+AF33*0.3</f>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="16"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+      <c r="AE33" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF33" s="16"/>
+      <c r="AG33" s="28">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4901,19 +4707,19 @@
     <mergeCell ref="L2:S2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:J33">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K33">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4927,7 +4733,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S33">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4941,7 +4747,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y33">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4955,7 +4761,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AE33">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4969,7 +4775,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG33">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4983,16 +4789,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:R33">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
-      <formula>60</formula>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+      <formula>0.1</formula>
+      <formula>59.9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ileri Java Hafta 4
</commit_message>
<xml_diff>
--- a/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
+++ b/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
   <si>
     <t>Adı</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>SINAV (%30)</t>
+  </si>
+  <si>
+    <t>RÜMEYSA</t>
+  </si>
+  <si>
+    <t>YILDIRIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -725,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -788,6 +797,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -810,12 +822,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -846,6 +860,64 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1160,11 +1232,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG81"/>
+  <dimension ref="A1:AH82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI9" sqref="AI9"/>
+      <selection pane="bottomLeft" activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1173,12 +1245,13 @@
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.77734375" style="1" customWidth="1"/>
     <col min="20" max="21" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1190,85 +1263,85 @@
     <col min="34" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:34" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="38"/>
-    </row>
-    <row r="2" spans="1:33" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="41"/>
+    </row>
+    <row r="2" spans="1:34" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35">
         <v>2</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="34"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="39" t="s">
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="39" t="s">
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="39" t="s">
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="41"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="19" t="s">
         <v>100</v>
       </c>
@@ -1276,7 +1349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>91</v>
       </c>
@@ -1377,7 +1450,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
@@ -1393,14 +1466,16 @@
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="18">
-        <f>100*SUM(D4:J4)/(2*A$2)</f>
-        <v>100</v>
+        <f t="shared" ref="K4:K34" si="0">100*SUM(D4:J4)/(2*A$2)</f>
+        <v>150</v>
       </c>
       <c r="L4" s="15">
         <v>100</v>
@@ -1408,14 +1483,16 @@
       <c r="M4" s="6">
         <v>100</v>
       </c>
-      <c r="N4" s="6"/>
+      <c r="N4" s="6">
+        <v>80</v>
+      </c>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="18">
-        <f>SUM(L4:R4)/(A$2)</f>
-        <v>100</v>
+        <f t="shared" ref="S4:S34" si="1">SUM(L4:R4)/(A$2)</f>
+        <v>140</v>
       </c>
       <c r="T4" s="15"/>
       <c r="U4" s="6"/>
@@ -1423,7 +1500,7 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="18">
-        <f>SUM(T4:X4)</f>
+        <f t="shared" ref="Y4:Y34" si="2">SUM(T4:X4)</f>
         <v>0</v>
       </c>
       <c r="Z4" s="15"/>
@@ -1432,16 +1509,16 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="18">
-        <f>SUM(Z4:AD4)</f>
+        <f t="shared" ref="AE4:AE34" si="3">SUM(Z4:AD4)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="15"/>
       <c r="AG4" s="24">
-        <f>K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AG4:AG34" si="4">K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>67</v>
       </c>
@@ -1457,14 +1534,16 @@
       <c r="E5" s="7">
         <v>2</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="18">
-        <f>100*SUM(D5:J5)/(2*A$2)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="L5" s="15">
         <v>100</v>
@@ -1472,14 +1551,16 @@
       <c r="M5" s="6">
         <v>80</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="6">
+        <v>80</v>
+      </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="18">
-        <f>SUM(L5:R5)/(A$2)</f>
-        <v>90</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="T5" s="15"/>
       <c r="U5" s="6"/>
@@ -1487,7 +1568,7 @@
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="18">
-        <f>SUM(T5:X5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z5" s="15"/>
@@ -1496,16 +1577,16 @@
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
       <c r="AE5" s="18">
-        <f>SUM(Z5:AD5)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF5" s="15"/>
       <c r="AG5" s="24">
-        <f>K5*0.1+S5*0.2+Y5*0.2+AE5*0.2+AF5*0.3</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>88</v>
       </c>
@@ -1521,14 +1602,16 @@
       <c r="E6" s="7">
         <v>1.7</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>1.7</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="18">
-        <f>100*SUM(D6:J6)/(2*A$2)</f>
-        <v>85</v>
+        <f t="shared" si="0"/>
+        <v>127.49999999999999</v>
       </c>
       <c r="L6" s="15">
         <v>90</v>
@@ -1536,14 +1619,16 @@
       <c r="M6" s="6">
         <v>100</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="6">
+        <v>100</v>
+      </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="18">
-        <f>SUM(L6:R6)/(A$2)</f>
-        <v>95</v>
+        <f t="shared" si="1"/>
+        <v>145</v>
       </c>
       <c r="T6" s="15"/>
       <c r="U6" s="6"/>
@@ -1551,7 +1636,7 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="18">
-        <f>SUM(T6:X6)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z6" s="15"/>
@@ -1560,16 +1645,19 @@
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="18">
-        <f>SUM(Z6:AD6)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF6" s="15"/>
       <c r="AG6" s="24">
-        <f>K6*0.1+S6*0.2+Y6*0.2+AE6*0.2+AF6*0.3</f>
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>41.75</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>73</v>
       </c>
@@ -1585,14 +1673,16 @@
       <c r="E7" s="7">
         <v>2</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="18">
-        <f>100*SUM(D7:J7)/(2*A$2)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="L7" s="15">
         <v>100</v>
@@ -1600,14 +1690,16 @@
       <c r="M7" s="6">
         <v>70</v>
       </c>
-      <c r="N7" s="6"/>
+      <c r="N7" s="6">
+        <v>60</v>
+      </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="18">
-        <f>SUM(L7:R7)/(A$2)</f>
-        <v>85</v>
+        <f t="shared" si="1"/>
+        <v>115</v>
       </c>
       <c r="T7" s="15"/>
       <c r="U7" s="6"/>
@@ -1615,7 +1707,7 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="18">
-        <f>SUM(T7:X7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z7" s="15"/>
@@ -1624,16 +1716,16 @@
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="18">
-        <f>SUM(Z7:AD7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF7" s="15"/>
       <c r="AG7" s="24">
-        <f>K7*0.1+S7*0.2+Y7*0.2+AE7*0.2+AF7*0.3</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>16</v>
       </c>
@@ -1649,13 +1741,15 @@
       <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="18">
-        <f>100*SUM(D8:J8)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L8" s="15">
@@ -1664,13 +1758,15 @@
       <c r="M8" s="6">
         <v>60</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="18">
-        <f>SUM(L8:R8)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="T8" s="15"/>
@@ -1679,7 +1775,7 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="18">
-        <f>SUM(T8:X8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z8" s="15"/>
@@ -1688,16 +1784,16 @@
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="18">
-        <f>SUM(Z8:AD8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF8" s="15"/>
       <c r="AG8" s="24">
-        <f>K8*0.1+S8*0.2+Y8*0.2+AE8*0.2+AF8*0.3</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>46</v>
       </c>
@@ -1713,14 +1809,16 @@
       <c r="E9" s="7">
         <v>2</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="18">
-        <f>100*SUM(D9:J9)/(2*A$2)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="L9" s="15">
         <v>100</v>
@@ -1728,14 +1826,16 @@
       <c r="M9" s="6">
         <v>60</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="N9" s="6">
+        <v>60</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="18">
-        <f>SUM(L9:R9)/(A$2)</f>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
       <c r="T9" s="15"/>
       <c r="U9" s="6"/>
@@ -1743,7 +1843,7 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="18">
-        <f>SUM(T9:X9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z9" s="15"/>
@@ -1752,16 +1852,16 @@
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
       <c r="AE9" s="18">
-        <f>SUM(Z9:AD9)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF9" s="15"/>
       <c r="AG9" s="24">
-        <f>K9*0.1+S9*0.2+Y9*0.2+AE9*0.2+AF9*0.3</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>52</v>
       </c>
@@ -1777,14 +1877,16 @@
       <c r="E10" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>1.9</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="18">
-        <f>100*SUM(D10:J10)/(2*A$2)</f>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>122.50000000000001</v>
       </c>
       <c r="L10" s="15">
         <v>100</v>
@@ -1792,14 +1894,16 @@
       <c r="M10" s="6">
         <v>0</v>
       </c>
-      <c r="N10" s="6"/>
+      <c r="N10" s="6">
+        <v>60</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="18">
-        <f>SUM(L10:R10)/(A$2)</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="T10" s="15"/>
       <c r="U10" s="6"/>
@@ -1807,7 +1911,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="18">
-        <f>SUM(T10:X10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z10" s="15"/>
@@ -1816,16 +1920,16 @@
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="18">
-        <f>SUM(Z10:AD10)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF10" s="15"/>
       <c r="AG10" s="24">
-        <f>K10*0.1+S10*0.2+Y10*0.2+AE10*0.2+AF10*0.3</f>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>28.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>58</v>
       </c>
@@ -1841,14 +1945,16 @@
       <c r="E11" s="7">
         <v>2</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="18">
-        <f>100*SUM(D11:J11)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L11" s="15">
         <v>0</v>
@@ -1856,14 +1962,16 @@
       <c r="M11" s="6">
         <v>100</v>
       </c>
-      <c r="N11" s="6"/>
+      <c r="N11" s="6">
+        <v>80</v>
+      </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="18">
-        <f>SUM(L11:R11)/(A$2)</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="6"/>
@@ -1871,7 +1979,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="18">
-        <f>SUM(T11:X11)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z11" s="15"/>
@@ -1880,16 +1988,16 @@
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
       <c r="AE11" s="18">
-        <f>SUM(Z11:AD11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF11" s="15"/>
       <c r="AG11" s="24">
-        <f>K11*0.1+S11*0.2+Y11*0.2+AE11*0.2+AF11*0.3</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>79</v>
       </c>
@@ -1905,14 +2013,16 @@
       <c r="E12" s="7">
         <v>2</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="18">
-        <f>100*SUM(D12:J12)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L12" s="15">
         <v>0</v>
@@ -1920,14 +2030,16 @@
       <c r="M12" s="6">
         <v>100</v>
       </c>
-      <c r="N12" s="6"/>
+      <c r="N12" s="6">
+        <v>100</v>
+      </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="18">
-        <f>SUM(L12:R12)/(A$2)</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="T12" s="15"/>
       <c r="U12" s="6"/>
@@ -1935,7 +2047,7 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="18">
-        <f>SUM(T12:X12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z12" s="15"/>
@@ -1944,16 +2056,16 @@
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="18">
-        <f>SUM(Z12:AD12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF12" s="15"/>
       <c r="AG12" s="24">
-        <f>K12*0.1+S12*0.2+Y12*0.2+AE12*0.2+AF12*0.3</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>82</v>
       </c>
@@ -1969,14 +2081,16 @@
       <c r="E13" s="7">
         <v>2</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="18">
-        <f>100*SUM(D13:J13)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L13" s="15">
         <v>0</v>
@@ -1984,14 +2098,16 @@
       <c r="M13" s="6">
         <v>100</v>
       </c>
-      <c r="N13" s="6"/>
+      <c r="N13" s="6">
+        <v>100</v>
+      </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="18">
-        <f>SUM(L13:R13)/(A$2)</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="6"/>
@@ -1999,7 +2115,7 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="18">
-        <f>SUM(T13:X13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z13" s="15"/>
@@ -2008,16 +2124,16 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="18">
-        <f>SUM(Z13:AD13)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF13" s="15"/>
       <c r="AG13" s="24">
-        <f>K13*0.1+S13*0.2+Y13*0.2+AE13*0.2+AF13*0.3</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>37</v>
       </c>
@@ -2033,13 +2149,15 @@
       <c r="E14" s="7">
         <v>2</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="18">
-        <f>100*SUM(D14:J14)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="L14" s="15">
@@ -2048,13 +2166,15 @@
       <c r="M14" s="6">
         <v>75</v>
       </c>
-      <c r="N14" s="6"/>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="18">
-        <f>SUM(L14:R14)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
       <c r="T14" s="15"/>
@@ -2063,7 +2183,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="18">
-        <f>SUM(T14:X14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z14" s="15"/>
@@ -2072,16 +2192,16 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="18">
-        <f>SUM(Z14:AD14)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF14" s="15"/>
       <c r="AG14" s="24">
-        <f>K14*0.1+S14*0.2+Y14*0.2+AE14*0.2+AF14*0.3</f>
+        <f t="shared" si="4"/>
         <v>12.5</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>31</v>
       </c>
@@ -2097,13 +2217,15 @@
       <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="18">
-        <f>100*SUM(D15:J15)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="L15" s="15">
@@ -2112,13 +2234,15 @@
       <c r="M15" s="6">
         <v>85</v>
       </c>
-      <c r="N15" s="6"/>
+      <c r="N15" s="6">
+        <v>0</v>
+      </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="18">
-        <f>SUM(L15:R15)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
       <c r="T15" s="15"/>
@@ -2127,7 +2251,7 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="18">
-        <f>SUM(T15:X15)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z15" s="15"/>
@@ -2136,16 +2260,16 @@
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="18">
-        <f>SUM(Z15:AD15)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF15" s="15"/>
       <c r="AG15" s="24">
-        <f>K15*0.1+S15*0.2+Y15*0.2+AE15*0.2+AF15*0.3</f>
+        <f t="shared" si="4"/>
         <v>12.25</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>8</v>
       </c>
@@ -2161,14 +2285,16 @@
       <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="18">
-        <f>100*SUM(D16:J16)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L16" s="15">
         <v>0</v>
@@ -2176,14 +2302,16 @@
       <c r="M16" s="6">
         <v>70</v>
       </c>
-      <c r="N16" s="6"/>
+      <c r="N16" s="6">
+        <v>60</v>
+      </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="18">
-        <f>SUM(L16:R16)/(A$2)</f>
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="T16" s="15"/>
       <c r="U16" s="6"/>
@@ -2191,7 +2319,7 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="18">
-        <f>SUM(T16:X16)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z16" s="15"/>
@@ -2200,13 +2328,13 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="18">
-        <f>SUM(Z16:AD16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF16" s="15"/>
       <c r="AG16" s="24">
-        <f>K16*0.1+S16*0.2+Y16*0.2+AE16*0.2+AF16*0.3</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2225,14 +2353,16 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>2</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="18">
-        <f>100*SUM(D17:J17)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L17" s="15">
         <v>0</v>
@@ -2240,14 +2370,16 @@
       <c r="M17" s="6">
         <v>70</v>
       </c>
-      <c r="N17" s="6"/>
+      <c r="N17" s="6">
+        <v>60</v>
+      </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="18">
-        <f>SUM(L17:R17)/(A$2)</f>
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="T17" s="15"/>
       <c r="U17" s="6"/>
@@ -2255,7 +2387,7 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="18">
-        <f>SUM(T17:X17)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z17" s="15"/>
@@ -2264,13 +2396,13 @@
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="18">
-        <f>SUM(Z17:AD17)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF17" s="15"/>
       <c r="AG17" s="24">
-        <f>K17*0.1+S17*0.2+Y17*0.2+AE17*0.2+AF17*0.3</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2289,13 +2421,15 @@
       <c r="E18" s="7">
         <v>2</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="18">
-        <f>100*SUM(D18:J18)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="L18" s="15">
@@ -2304,13 +2438,15 @@
       <c r="M18" s="6">
         <v>60</v>
       </c>
-      <c r="N18" s="6"/>
+      <c r="N18" s="6">
+        <v>0</v>
+      </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="18">
-        <f>SUM(L18:R18)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="T18" s="15"/>
@@ -2319,7 +2455,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="18">
-        <f>SUM(T18:X18)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z18" s="15"/>
@@ -2328,12 +2464,12 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="18">
-        <f>SUM(Z18:AD18)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF18" s="15"/>
       <c r="AG18" s="24">
-        <f>K18*0.1+S18*0.2+Y18*0.2+AE18*0.2+AF18*0.3</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -2353,13 +2489,15 @@
       <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="18">
-        <f>100*SUM(D19:J19)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="L19" s="15">
@@ -2368,13 +2506,15 @@
       <c r="M19" s="6">
         <v>60</v>
       </c>
-      <c r="N19" s="6"/>
+      <c r="N19" s="6">
+        <v>0</v>
+      </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="18">
-        <f>SUM(L19:R19)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="T19" s="15"/>
@@ -2383,7 +2523,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="18">
-        <f>SUM(T19:X19)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z19" s="15"/>
@@ -2392,12 +2532,12 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="18">
-        <f>SUM(Z19:AD19)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF19" s="15"/>
       <c r="AG19" s="24">
-        <f>K19*0.1+S19*0.2+Y19*0.2+AE19*0.2+AF19*0.3</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -2417,13 +2557,15 @@
       <c r="E20" s="7">
         <v>2</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="18">
-        <f>100*SUM(D20:J20)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="L20" s="15">
@@ -2432,13 +2574,15 @@
       <c r="M20" s="6">
         <v>60</v>
       </c>
-      <c r="N20" s="6"/>
+      <c r="N20" s="6">
+        <v>0</v>
+      </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="18">
-        <f>SUM(L20:R20)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="T20" s="15"/>
@@ -2447,7 +2591,7 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="18">
-        <f>SUM(T20:X20)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z20" s="15"/>
@@ -2456,12 +2600,12 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="18">
-        <f>SUM(Z20:AD20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF20" s="15"/>
       <c r="AG20" s="24">
-        <f>K20*0.1+S20*0.2+Y20*0.2+AE20*0.2+AF20*0.3</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -2481,14 +2625,16 @@
       <c r="E21" s="7">
         <v>2</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>2</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="18">
-        <f>100*SUM(D21:J21)/(2*A$2)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L21" s="15">
         <v>0</v>
@@ -2496,14 +2642,16 @@
       <c r="M21" s="6">
         <v>50</v>
       </c>
-      <c r="N21" s="6"/>
+      <c r="N21" s="6">
+        <v>70</v>
+      </c>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="18">
-        <f>SUM(L21:R21)/(A$2)</f>
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="T21" s="15"/>
       <c r="U21" s="6"/>
@@ -2511,7 +2659,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
       <c r="Y21" s="18">
-        <f>SUM(T21:X21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z21" s="15"/>
@@ -2520,13 +2668,13 @@
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="18">
-        <f>SUM(Z21:AD21)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF21" s="15"/>
       <c r="AG21" s="24">
-        <f>K21*0.1+S21*0.2+Y21*0.2+AE21*0.2+AF21*0.3</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,13 +2693,15 @@
       <c r="E22" s="7">
         <v>0</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="18">
-        <f>100*SUM(D22:J22)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L22" s="15">
@@ -2560,13 +2710,15 @@
       <c r="M22" s="6">
         <v>0</v>
       </c>
-      <c r="N22" s="6"/>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="18">
-        <f>SUM(L22:R22)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T22" s="15"/>
@@ -2575,7 +2727,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="18">
-        <f>SUM(T22:X22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z22" s="15"/>
@@ -2584,12 +2736,12 @@
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="18">
-        <f>SUM(Z22:AD22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF22" s="15"/>
       <c r="AG22" s="24">
-        <f>K22*0.1+S22*0.2+Y22*0.2+AE22*0.2+AF22*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2609,14 +2761,16 @@
       <c r="E23" s="7">
         <v>0</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="18">
-        <f>100*SUM(D23:J23)/(2*A$2)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="L23" s="15">
         <v>0</v>
@@ -2624,13 +2778,15 @@
       <c r="M23" s="6">
         <v>0</v>
       </c>
-      <c r="N23" s="6"/>
+      <c r="N23" s="6">
+        <v>0</v>
+      </c>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="18">
-        <f>SUM(L23:R23)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T23" s="15"/>
@@ -2639,7 +2795,7 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
       <c r="Y23" s="18">
-        <f>SUM(T23:X23)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z23" s="15"/>
@@ -2648,13 +2804,13 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
       <c r="AE23" s="18">
-        <f>SUM(Z23:AD23)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF23" s="15"/>
       <c r="AG23" s="24">
-        <f>K23*0.1+S23*0.2+Y23*0.2+AE23*0.2+AF23*0.3</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2673,13 +2829,15 @@
       <c r="E24" s="7">
         <v>0</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="18">
-        <f>100*SUM(D24:J24)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" s="15">
@@ -2688,13 +2846,15 @@
       <c r="M24" s="6">
         <v>0</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="18">
-        <f>SUM(L24:R24)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T24" s="15"/>
@@ -2703,7 +2863,7 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="18">
-        <f>SUM(T24:X24)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z24" s="15"/>
@@ -2712,12 +2872,12 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
       <c r="AE24" s="18">
-        <f>SUM(Z24:AD24)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF24" s="15"/>
       <c r="AG24" s="24">
-        <f>K24*0.1+S24*0.2+Y24*0.2+AE24*0.2+AF24*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2737,13 +2897,15 @@
       <c r="E25" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="18">
-        <f>100*SUM(D25:J25)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25" s="15">
@@ -2752,13 +2914,15 @@
       <c r="M25" s="6">
         <v>0</v>
       </c>
-      <c r="N25" s="6"/>
+      <c r="N25" s="6">
+        <v>0</v>
+      </c>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="18">
-        <f>SUM(L25:R25)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T25" s="15"/>
@@ -2767,7 +2931,7 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
       <c r="Y25" s="18">
-        <f>SUM(T25:X25)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z25" s="15"/>
@@ -2776,12 +2940,12 @@
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
       <c r="AE25" s="18">
-        <f>SUM(Z25:AD25)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF25" s="15"/>
       <c r="AG25" s="24">
-        <f>K25*0.1+S25*0.2+Y25*0.2+AE25*0.2+AF25*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2796,19 +2960,21 @@
         <v>27</v>
       </c>
       <c r="D26" s="12">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="18">
-        <f>100*SUM(D26:J26)/(2*A$2)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>75</v>
       </c>
       <c r="L26" s="15">
         <v>0</v>
@@ -2816,14 +2982,16 @@
       <c r="M26" s="6">
         <v>0</v>
       </c>
-      <c r="N26" s="6"/>
+      <c r="N26" s="6">
+        <v>60</v>
+      </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="18">
-        <f>SUM(L26:R26)/(A$2)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="T26" s="15"/>
       <c r="U26" s="6"/>
@@ -2831,7 +2999,7 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="18">
-        <f>SUM(T26:X26)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z26" s="15"/>
@@ -2840,13 +3008,13 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="18">
-        <f>SUM(Z26:AD26)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF26" s="15"/>
       <c r="AG26" s="24">
-        <f>K26*0.1+S26*0.2+Y26*0.2+AE26*0.2+AF26*0.3</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>13.5</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2865,13 +3033,15 @@
       <c r="E27" s="7">
         <v>0</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="18">
-        <f>100*SUM(D27:J27)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27" s="15">
@@ -2880,13 +3050,15 @@
       <c r="M27" s="6">
         <v>0</v>
       </c>
-      <c r="N27" s="6"/>
+      <c r="N27" s="6">
+        <v>0</v>
+      </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="18">
-        <f>SUM(L27:R27)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T27" s="15"/>
@@ -2895,7 +3067,7 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="18">
-        <f>SUM(T27:X27)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z27" s="15"/>
@@ -2904,12 +3076,12 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
       <c r="AE27" s="18">
-        <f>SUM(Z27:AD27)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF27" s="15"/>
       <c r="AG27" s="24">
-        <f>K27*0.1+S27*0.2+Y27*0.2+AE27*0.2+AF27*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2929,13 +3101,15 @@
       <c r="E28" s="7">
         <v>0</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="18">
-        <f>100*SUM(D28:J28)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" s="15">
@@ -2944,13 +3118,15 @@
       <c r="M28" s="6">
         <v>0</v>
       </c>
-      <c r="N28" s="6"/>
+      <c r="N28" s="6">
+        <v>0</v>
+      </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="18">
-        <f>SUM(L28:R28)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T28" s="15"/>
@@ -2959,7 +3135,7 @@
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
       <c r="Y28" s="18">
-        <f>SUM(T28:X28)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z28" s="15"/>
@@ -2968,12 +3144,12 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
       <c r="AE28" s="18">
-        <f>SUM(Z28:AD28)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF28" s="15"/>
       <c r="AG28" s="24">
-        <f>K28*0.1+S28*0.2+Y28*0.2+AE28*0.2+AF28*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2993,13 +3169,15 @@
       <c r="E29" s="7">
         <v>0</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="18">
-        <f>100*SUM(D29:J29)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L29" s="15">
@@ -3008,13 +3186,15 @@
       <c r="M29" s="6">
         <v>0</v>
       </c>
-      <c r="N29" s="6"/>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="18">
-        <f>SUM(L29:R29)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T29" s="15"/>
@@ -3023,7 +3203,7 @@
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
       <c r="Y29" s="18">
-        <f>SUM(T29:X29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z29" s="15"/>
@@ -3032,12 +3212,12 @@
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
       <c r="AE29" s="18">
-        <f>SUM(Z29:AD29)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF29" s="15"/>
       <c r="AG29" s="24">
-        <f>K29*0.1+S29*0.2+Y29*0.2+AE29*0.2+AF29*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3057,13 +3237,15 @@
       <c r="E30" s="7">
         <v>0</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="18">
-        <f>100*SUM(D30:J30)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L30" s="15">
@@ -3072,13 +3254,15 @@
       <c r="M30" s="6">
         <v>0</v>
       </c>
-      <c r="N30" s="6"/>
+      <c r="N30" s="6">
+        <v>0</v>
+      </c>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="18">
-        <f>SUM(L30:R30)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T30" s="15"/>
@@ -3087,7 +3271,7 @@
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="18">
-        <f>SUM(T30:X30)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z30" s="15"/>
@@ -3096,12 +3280,12 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
       <c r="AE30" s="18">
-        <f>SUM(Z30:AD30)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF30" s="15"/>
       <c r="AG30" s="24">
-        <f>K30*0.1+S30*0.2+Y30*0.2+AE30*0.2+AF30*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3121,13 +3305,15 @@
       <c r="E31" s="7">
         <v>0</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="18">
-        <f>100*SUM(D31:J31)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L31" s="15">
@@ -3136,13 +3322,15 @@
       <c r="M31" s="6">
         <v>0</v>
       </c>
-      <c r="N31" s="6"/>
+      <c r="N31" s="6">
+        <v>0</v>
+      </c>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="18">
-        <f>SUM(L31:R31)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T31" s="15"/>
@@ -3151,7 +3339,7 @@
       <c r="W31" s="6"/>
       <c r="X31" s="6"/>
       <c r="Y31" s="18">
-        <f>SUM(T31:X31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z31" s="15"/>
@@ -3160,12 +3348,12 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
       <c r="AE31" s="18">
-        <f>SUM(Z31:AD31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF31" s="15"/>
       <c r="AG31" s="24">
-        <f>K31*0.1+S31*0.2+Y31*0.2+AE31*0.2+AF31*0.3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3185,13 +3373,15 @@
       <c r="E32" s="7">
         <v>0</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="18">
-        <f>100*SUM(D32:J32)/(2*A$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L32" s="15">
@@ -3200,13 +3390,15 @@
       <c r="M32" s="6">
         <v>0</v>
       </c>
-      <c r="N32" s="6"/>
+      <c r="N32" s="6">
+        <v>0</v>
+      </c>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="18">
-        <f>SUM(L32:R32)/(A$2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T32" s="15"/>
@@ -3215,7 +3407,7 @@
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="18">
-        <f>SUM(T32:X32)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z32" s="15"/>
@@ -3224,89 +3416,150 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
       <c r="AE32" s="18">
-        <f>SUM(Z32:AD32)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF32" s="15"/>
       <c r="AG32" s="24">
-        <f>K32*0.1+S32*0.2+Y32*0.2+AE32*0.2+AF32*0.3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:33" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="18">
+        <f t="shared" ref="K33" si="5">100*SUM(D33:J33)/(2*A$2)</f>
+        <v>50</v>
+      </c>
+      <c r="L33" s="15">
+        <v>0</v>
+      </c>
+      <c r="M33" s="6">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6">
+        <v>60</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="18">
+        <f t="shared" ref="S33" si="6">SUM(L33:R33)/(A$2)</f>
+        <v>30</v>
+      </c>
+      <c r="T33" s="15"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="18">
+        <f t="shared" ref="Y33" si="7">SUM(T33:X33)</f>
+        <v>0</v>
+      </c>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="6"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6"/>
+      <c r="AE33" s="18">
+        <f t="shared" ref="AE33" si="8">SUM(Z33:AD33)</f>
+        <v>0</v>
+      </c>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="24">
+        <f t="shared" ref="AG33" si="9">K33*0.1+S33*0.2+Y33*0.2+AE33*0.2+AF33*0.3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B34" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C34" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="13">
-        <v>0</v>
-      </c>
-      <c r="E33" s="14">
-        <v>0</v>
-      </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="18">
-        <f>100*SUM(D33:J33)/(2*A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="15">
-        <v>0</v>
-      </c>
-      <c r="M33" s="6">
-        <v>0</v>
-      </c>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="18">
-        <f>SUM(L33:R33)/(A$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T33" s="16"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="17"/>
-      <c r="X33" s="17"/>
-      <c r="Y33" s="20">
-        <f>SUM(T33:X33)</f>
-        <v>0</v>
-      </c>
-      <c r="Z33" s="16"/>
-      <c r="AA33" s="17"/>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="18">
-        <f>SUM(Z33:AD33)</f>
-        <v>0</v>
-      </c>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="28">
-        <f>K33*0.1+S33*0.2+Y33*0.2+AE33*0.2+AF33*0.3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:33" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="13">
+        <v>0</v>
+      </c>
+      <c r="E34" s="14">
+        <v>0</v>
+      </c>
+      <c r="F34" s="14">
+        <v>0</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="15">
+        <v>0</v>
+      </c>
+      <c r="M34" s="6">
+        <v>0</v>
+      </c>
+      <c r="N34" s="17">
+        <v>0</v>
+      </c>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T34" s="16"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z34" s="16"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF34" s="16"/>
+      <c r="AG34" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3314,24 +3567,6 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
     </row>
     <row r="36" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
@@ -4575,6 +4810,33 @@
       <c r="X81" s="9"/>
       <c r="Y81" s="9"/>
     </row>
+    <row r="82" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
+      <c r="R82" s="9"/>
+      <c r="S82" s="9"/>
+      <c r="T82" s="9"/>
+      <c r="U82" s="9"/>
+      <c r="V82" s="9"/>
+      <c r="W82" s="9"/>
+      <c r="X82" s="9"/>
+      <c r="Y82" s="9"/>
+    </row>
   </sheetData>
   <sortState ref="A4:AG33">
     <sortCondition descending="1" ref="AG4:AG33"/>
@@ -4586,19 +4848,19 @@
     <mergeCell ref="D2:K2"/>
     <mergeCell ref="L2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:J33">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="between">
+  <conditionalFormatting sqref="D4:J34">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K33">
+  <conditionalFormatting sqref="K4:K34">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
@@ -4612,7 +4874,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S33">
+  <conditionalFormatting sqref="S4:S34">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
@@ -4626,7 +4888,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y4:Y33">
+  <conditionalFormatting sqref="Y4:Y34">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -4640,7 +4902,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE4:AE33">
+  <conditionalFormatting sqref="AE4:AE34">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -4654,7 +4916,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG4:AG33">
+  <conditionalFormatting sqref="AG4:AG34">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
@@ -4668,21 +4930,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:R33">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
-      <formula>80</formula>
-      <formula>100</formula>
+  <conditionalFormatting sqref="L4:R34">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
+      <formula>0.1</formula>
+      <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>0.1</formula>
-      <formula>59.9</formula>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+      <formula>80</formula>
+      <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4700,7 +4962,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K4:K33</xm:sqref>
+          <xm:sqref>K4:K34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1E54EB9-FD52-4CFD-8B29-7F3B7B6681D5}">
@@ -4711,7 +4973,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S4:S33</xm:sqref>
+          <xm:sqref>S4:S34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{03C5F189-3F43-4B84-A0F5-49F108E9F2B6}">
@@ -4722,7 +4984,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Y4:Y33</xm:sqref>
+          <xm:sqref>Y4:Y34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{04C393DA-4C35-49B7-B05F-92E59E130F0F}">
@@ -4733,7 +4995,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>AE4:AE33</xm:sqref>
+          <xm:sqref>AE4:AE34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43DC70F4-8291-4430-AFF0-577FC5E79CD9}">
@@ -4744,7 +5006,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>AG4:AG33</xm:sqref>
+          <xm:sqref>AG4:AG34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Hafta 6 not guncelleme
</commit_message>
<xml_diff>
--- a/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
+++ b/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
@@ -782,7 +782,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1173,8 +1211,8 @@
   <dimension ref="A1:AH81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1188,8 +1226,8 @@
     <col min="10" max="10" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.5546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="4.77734375" style="1" customWidth="1"/>
     <col min="20" max="21" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1377,12 +1415,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="18">
-        <f t="shared" ref="K3:K33" si="0">100*SUM(D3:J3)/(2*A$1)</f>
-        <v>144.99999999999997</v>
+        <f>100*SUM(D3:J3)/(2*A$1)</f>
+        <v>161.66666666666666</v>
       </c>
       <c r="L3" s="15">
         <v>90</v>
@@ -1399,11 +1437,13 @@
       <c r="P3" s="6">
         <v>95</v>
       </c>
-      <c r="Q3" s="6"/>
+      <c r="Q3" s="6">
+        <v>100</v>
+      </c>
       <c r="R3" s="6"/>
       <c r="S3" s="18">
-        <f t="shared" ref="S3:S33" si="1">SUM(L3:R3)/(A$1)</f>
-        <v>160</v>
+        <f>SUM(L3:R3)/(A$1)</f>
+        <v>193.33333333333334</v>
       </c>
       <c r="T3" s="15">
         <v>60</v>
@@ -1415,7 +1455,7 @@
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="18">
-        <f t="shared" ref="Y3:Y33" si="2">SUM(T3:X3)</f>
+        <f>SUM(T3:X3)</f>
         <v>120</v>
       </c>
       <c r="Z3" s="15"/>
@@ -1424,13 +1464,13 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="18">
-        <f t="shared" ref="AE3:AE33" si="3">SUM(Z3:AD3)</f>
+        <f>SUM(Z3:AD3)</f>
         <v>0</v>
       </c>
       <c r="AF3" s="15"/>
       <c r="AG3" s="24">
-        <f t="shared" ref="AG3:AG33" si="4">K3*0.1+S3*0.2+Y3*0.2+AE3*0.2+AF3*0.3</f>
-        <v>70.5</v>
+        <f>K3*0.1+S3*0.2+Y3*0.2+AE3*0.2+AF3*0.3</f>
+        <v>78.833333333333343</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>103</v>
@@ -1438,16 +1478,16 @@
     </row>
     <row r="4" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D4" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
         <v>2</v>
@@ -1461,32 +1501,36 @@
       <c r="H4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D4:J4)/(2*A$1)</f>
         <v>166.66666666666666</v>
       </c>
       <c r="L4" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M4" s="6">
         <v>100</v>
       </c>
       <c r="N4" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O4" s="6">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="P4" s="6">
-        <v>70</v>
-      </c>
-      <c r="Q4" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>95</v>
+      </c>
       <c r="R4" s="6"/>
       <c r="S4" s="18">
-        <f t="shared" si="1"/>
-        <v>136.66666666666666</v>
+        <f>SUM(L4:R4)/(A$1)</f>
+        <v>165</v>
       </c>
       <c r="T4" s="15">
         <v>60</v>
@@ -1498,7 +1542,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T4:X4)</f>
         <v>120</v>
       </c>
       <c r="Z4" s="15"/>
@@ -1507,24 +1551,24 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z4:AD4)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="15"/>
       <c r="AG4" s="24">
-        <f t="shared" si="4"/>
-        <v>68</v>
+        <f>K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
+        <v>73.666666666666671</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D5" s="12">
         <v>2</v>
@@ -1536,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="7">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
@@ -1546,14 +1590,14 @@
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="18">
-        <f t="shared" si="0"/>
-        <v>173.33333333333334</v>
+        <f>100*SUM(D5:J5)/(2*A$1)</f>
+        <v>183.33333333333334</v>
       </c>
       <c r="L5" s="15">
         <v>100</v>
       </c>
       <c r="M5" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N5" s="6">
         <v>80</v>
@@ -1562,22 +1606,28 @@
         <v>60</v>
       </c>
       <c r="P5" s="6">
-        <v>100</v>
-      </c>
-      <c r="Q5" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>50</v>
+      </c>
       <c r="R5" s="6"/>
       <c r="S5" s="18">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
+        <f>SUM(L5:R5)/(A$1)</f>
+        <v>153.33333333333334</v>
+      </c>
+      <c r="T5" s="15">
+        <v>60</v>
+      </c>
+      <c r="U5" s="15">
+        <v>60</v>
+      </c>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
       <c r="Y5" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(T5:X5)</f>
+        <v>120</v>
       </c>
       <c r="Z5" s="15"/>
       <c r="AA5" s="6"/>
@@ -1585,27 +1635,27 @@
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
       <c r="AE5" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z5:AD5)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="15"/>
       <c r="AG5" s="24">
-        <f t="shared" si="4"/>
-        <v>45.333333333333336</v>
+        <f>K5*0.1+S5*0.2+Y5*0.2+AE5*0.2+AF5*0.3</f>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D6" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="7">
         <v>2</v>
@@ -1617,45 +1667,51 @@
         <v>2</v>
       </c>
       <c r="H6" s="7">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="I6" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="18">
-        <f t="shared" si="0"/>
-        <v>180</v>
+        <f>100*SUM(D6:J6)/(2*A$1)</f>
+        <v>161.66666666666666</v>
       </c>
       <c r="L6" s="15">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
         <v>100</v>
       </c>
-      <c r="M6" s="6">
-        <v>70</v>
-      </c>
       <c r="N6" s="6">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="O6" s="6">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="P6" s="6">
-        <v>70</v>
-      </c>
-      <c r="Q6" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>90</v>
+      </c>
       <c r="R6" s="6"/>
       <c r="S6" s="18">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
+        <f>SUM(L6:R6)/(A$1)</f>
+        <v>158.33333333333334</v>
+      </c>
+      <c r="T6" s="15">
+        <v>60</v>
+      </c>
+      <c r="U6" s="15">
+        <v>60</v>
+      </c>
       <c r="V6" s="15"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
       <c r="Y6" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(T6:X6)</f>
+        <v>120</v>
       </c>
       <c r="Z6" s="15"/>
       <c r="AA6" s="6"/>
@@ -1663,27 +1719,27 @@
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z6:AD6)</f>
         <v>0</v>
       </c>
       <c r="AF6" s="15"/>
       <c r="AG6" s="24">
-        <f t="shared" si="4"/>
-        <v>42</v>
+        <f>K6*0.1+S6*0.2+Y6*0.2+AE6*0.2+AF6*0.3</f>
+        <v>71.833333333333343</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D7" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -1698,35 +1754,39 @@
         <v>2</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="18">
-        <f t="shared" si="0"/>
-        <v>183.33333333333334</v>
+        <f>100*SUM(D7:J7)/(2*A$1)</f>
+        <v>166.66666666666666</v>
       </c>
       <c r="L7" s="15">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
         <v>100</v>
       </c>
-      <c r="M7" s="6">
-        <v>60</v>
-      </c>
       <c r="N7" s="6">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="O7" s="6">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="P7" s="6">
-        <v>90</v>
-      </c>
-      <c r="Q7" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>95</v>
+      </c>
       <c r="R7" s="6"/>
       <c r="S7" s="18">
-        <f t="shared" si="1"/>
-        <v>123.33333333333333</v>
-      </c>
-      <c r="T7" s="15"/>
+        <f>SUM(L7:R7)/(A$1)</f>
+        <v>153.33333333333334</v>
+      </c>
+      <c r="T7" s="15">
+        <v>60</v>
+      </c>
       <c r="U7" s="15">
         <v>60</v>
       </c>
@@ -1734,8 +1794,8 @@
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="18">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>SUM(T7:X7)</f>
+        <v>120</v>
       </c>
       <c r="Z7" s="15"/>
       <c r="AA7" s="6"/>
@@ -1743,27 +1803,27 @@
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
       <c r="AE7" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z7:AD7)</f>
         <v>0</v>
       </c>
       <c r="AF7" s="15"/>
       <c r="AG7" s="24">
-        <f t="shared" si="4"/>
-        <v>55</v>
+        <f>K7*0.1+S7*0.2+Y7*0.2+AE7*0.2+AF7*0.3</f>
+        <v>71.333333333333343</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D8" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
@@ -1778,37 +1838,37 @@
         <v>2</v>
       </c>
       <c r="I8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="18">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>100*SUM(D8:J8)/(2*A$1)</f>
+        <v>200</v>
       </c>
       <c r="L8" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M8" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N8" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O8" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="P8" s="6">
-        <v>100</v>
-      </c>
-      <c r="Q8" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>90</v>
+      </c>
       <c r="R8" s="6"/>
       <c r="S8" s="18">
-        <f t="shared" si="1"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="T8" s="15">
-        <v>60</v>
-      </c>
+        <f>SUM(L8:R8)/(A$1)</f>
+        <v>153.33333333333334</v>
+      </c>
+      <c r="T8" s="15"/>
       <c r="U8" s="15">
         <v>60</v>
       </c>
@@ -1816,8 +1876,8 @@
       <c r="W8" s="15"/>
       <c r="X8" s="15"/>
       <c r="Y8" s="18">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f>SUM(T8:X8)</f>
+        <v>60</v>
       </c>
       <c r="Z8" s="15"/>
       <c r="AA8" s="6"/>
@@ -1825,27 +1885,27 @@
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z8:AD8)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="15"/>
       <c r="AG8" s="24">
-        <f t="shared" si="4"/>
-        <v>65.666666666666671</v>
+        <f>K8*0.1+S8*0.2+Y8*0.2+AE8*0.2+AF8*0.3</f>
+        <v>62.666666666666671</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
@@ -1854,52 +1914,50 @@
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="H9" s="7">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="I9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="18">
-        <f t="shared" si="0"/>
-        <v>144.99999999999997</v>
+        <f>100*SUM(D9:J9)/(2*A$1)</f>
+        <v>190</v>
       </c>
       <c r="L9" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M9" s="6">
+        <v>80</v>
+      </c>
+      <c r="N9" s="6">
+        <v>80</v>
+      </c>
+      <c r="O9" s="6">
+        <v>60</v>
+      </c>
+      <c r="P9" s="6">
         <v>100</v>
       </c>
-      <c r="N9" s="6">
-        <v>100</v>
-      </c>
-      <c r="O9" s="6">
+      <c r="Q9" s="6">
         <v>95</v>
       </c>
-      <c r="P9" s="6">
-        <v>90</v>
-      </c>
-      <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="18">
-        <f t="shared" si="1"/>
-        <v>128.33333333333334</v>
-      </c>
-      <c r="T9" s="15">
-        <v>60</v>
-      </c>
-      <c r="U9" s="15">
-        <v>60</v>
-      </c>
+        <f>SUM(L9:R9)/(A$1)</f>
+        <v>171.66666666666666</v>
+      </c>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="18">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f>SUM(T9:X9)</f>
+        <v>0</v>
       </c>
       <c r="Z9" s="15"/>
       <c r="AA9" s="6"/>
@@ -1907,24 +1965,24 @@
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
       <c r="AE9" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z9:AD9)</f>
         <v>0</v>
       </c>
       <c r="AF9" s="15"/>
       <c r="AG9" s="24">
-        <f t="shared" si="4"/>
-        <v>64.166666666666671</v>
+        <f>K9*0.1+S9*0.2+Y9*0.2+AE9*0.2+AF9*0.3</f>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -1933,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="7">
         <v>2</v>
@@ -1942,37 +2000,37 @@
         <v>2</v>
       </c>
       <c r="I10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="18">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>100*SUM(D10:J10)/(2*A$1)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="L10" s="15">
         <v>0</v>
       </c>
       <c r="M10" s="6">
+        <v>75</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
         <v>100</v>
       </c>
-      <c r="N10" s="6">
-        <v>80</v>
-      </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <v>90</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>95</v>
       </c>
-      <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="18">
-        <f t="shared" si="1"/>
-        <v>121.66666666666667</v>
-      </c>
-      <c r="T10" s="15">
-        <v>60</v>
-      </c>
+        <f>SUM(L10:R10)/(A$1)</f>
+        <v>120</v>
+      </c>
+      <c r="T10" s="15"/>
       <c r="U10" s="15">
         <v>60</v>
       </c>
@@ -1980,8 +2038,8 @@
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="18">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f>SUM(T10:X10)</f>
+        <v>60</v>
       </c>
       <c r="Z10" s="15"/>
       <c r="AA10" s="6"/>
@@ -1989,51 +2047,53 @@
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z10:AD10)</f>
         <v>0</v>
       </c>
       <c r="AF10" s="15"/>
       <c r="AG10" s="24">
-        <f t="shared" si="4"/>
-        <v>63.333333333333336</v>
+        <f>K10*0.1+S10*0.2+Y10*0.2+AE10*0.2+AF10*0.3</f>
+        <v>49.333333333333336</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D11" s="12">
         <v>2</v>
       </c>
       <c r="E11" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="7">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="G11" s="7">
         <v>2</v>
       </c>
       <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>2</v>
+      </c>
       <c r="J11" s="7"/>
       <c r="K11" s="18">
-        <f t="shared" si="0"/>
-        <v>131.66666666666666</v>
+        <f>100*SUM(D11:J11)/(2*A$1)</f>
+        <v>196.66666666666666</v>
       </c>
       <c r="L11" s="15">
         <v>100</v>
       </c>
       <c r="M11" s="6">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N11" s="6">
         <v>60</v>
@@ -2042,13 +2102,15 @@
         <v>60</v>
       </c>
       <c r="P11" s="6">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>80</v>
+      </c>
       <c r="R11" s="6"/>
       <c r="S11" s="18">
-        <f t="shared" si="1"/>
-        <v>76.666666666666671</v>
+        <f>SUM(L11:R11)/(A$1)</f>
+        <v>146.66666666666666</v>
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
@@ -2056,7 +2118,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T11:X11)</f>
         <v>0</v>
       </c>
       <c r="Z11" s="15"/>
@@ -2065,24 +2127,24 @@
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
       <c r="AE11" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z11:AD11)</f>
         <v>0</v>
       </c>
       <c r="AF11" s="15"/>
       <c r="AG11" s="24">
-        <f t="shared" si="4"/>
-        <v>28.5</v>
+        <f>K11*0.1+S11*0.2+Y11*0.2+AE11*0.2+AF11*0.3</f>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D12" s="12">
         <v>0</v>
@@ -2091,51 +2153,55 @@
         <v>2</v>
       </c>
       <c r="F12" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="7">
         <v>2</v>
       </c>
       <c r="H12" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D12:J12)/(2*A$1)</f>
         <v>133.33333333333334</v>
       </c>
       <c r="L12" s="15">
         <v>0</v>
       </c>
       <c r="M12" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="N12" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O12" s="6">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="P12" s="6">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>95</v>
+      </c>
       <c r="R12" s="6"/>
       <c r="S12" s="18">
-        <f t="shared" si="1"/>
-        <v>66.666666666666671</v>
+        <f>SUM(L12:R12)/(A$1)</f>
+        <v>113.33333333333333</v>
       </c>
       <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
+      <c r="U12" s="15">
+        <v>60</v>
+      </c>
       <c r="V12" s="15"/>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(T12:X12)</f>
+        <v>60</v>
       </c>
       <c r="Z12" s="15"/>
       <c r="AA12" s="6"/>
@@ -2143,13 +2209,13 @@
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z12:AD12)</f>
         <v>0</v>
       </c>
       <c r="AF12" s="15"/>
       <c r="AG12" s="24">
-        <f t="shared" si="4"/>
-        <v>26.666666666666671</v>
+        <f>K12*0.1+S12*0.2+Y12*0.2+AE12*0.2+AF12*0.3</f>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,12 +2244,12 @@
         <v>1</v>
       </c>
       <c r="I13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="18">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
+        <f>100*SUM(D13:J13)/(2*A$1)</f>
+        <v>150</v>
       </c>
       <c r="L13" s="15">
         <v>0</v>
@@ -2200,11 +2266,13 @@
       <c r="P13" s="6">
         <v>20</v>
       </c>
-      <c r="Q13" s="6"/>
+      <c r="Q13" s="6">
+        <v>70</v>
+      </c>
       <c r="R13" s="6"/>
       <c r="S13" s="18">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f>SUM(L13:R13)/(A$1)</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
@@ -2212,7 +2280,7 @@
       <c r="W13" s="15"/>
       <c r="X13" s="15"/>
       <c r="Y13" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T13:X13)</f>
         <v>0</v>
       </c>
       <c r="Z13" s="15"/>
@@ -2221,24 +2289,24 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z13:AD13)</f>
         <v>0</v>
       </c>
       <c r="AF13" s="15"/>
       <c r="AG13" s="24">
-        <f t="shared" si="4"/>
-        <v>27.333333333333336</v>
+        <f>K13*0.1+S13*0.2+Y13*0.2+AE13*0.2+AF13*0.3</f>
+        <v>33.666666666666671</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
@@ -2253,34 +2321,38 @@
         <v>2</v>
       </c>
       <c r="H14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="18">
-        <f t="shared" si="0"/>
-        <v>116.66666666666667</v>
+        <f>100*SUM(D14:J14)/(2*A$1)</f>
+        <v>150</v>
       </c>
       <c r="L14" s="15">
         <v>0</v>
       </c>
       <c r="M14" s="6">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="N14" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="O14" s="6">
         <v>60</v>
       </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="P14" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>65</v>
+      </c>
       <c r="R14" s="6"/>
       <c r="S14" s="18">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f>SUM(L14:R14)/(A$1)</f>
+        <v>88.333333333333329</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
@@ -2288,7 +2360,7 @@
       <c r="W14" s="15"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T14:X14)</f>
         <v>0</v>
       </c>
       <c r="Z14" s="15"/>
@@ -2297,24 +2369,24 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z14:AD14)</f>
         <v>0</v>
       </c>
       <c r="AF14" s="15"/>
       <c r="AG14" s="24">
-        <f t="shared" si="4"/>
-        <v>23.666666666666668</v>
+        <f>K14*0.1+S14*0.2+Y14*0.2+AE14*0.2+AF14*0.3</f>
+        <v>32.666666666666671</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -2323,53 +2395,53 @@
         <v>2</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="7">
         <v>2</v>
       </c>
       <c r="H15" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="18">
-        <f t="shared" si="0"/>
-        <v>116.66666666666667</v>
+        <f>100*SUM(D15:J15)/(2*A$1)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="L15" s="15">
         <v>0</v>
       </c>
       <c r="M15" s="6">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="N15" s="6">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="O15" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="P15" s="6">
-        <v>90</v>
-      </c>
-      <c r="Q15" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>95</v>
+      </c>
       <c r="R15" s="6"/>
       <c r="S15" s="18">
-        <f t="shared" si="1"/>
-        <v>88.333333333333329</v>
+        <f>SUM(L15:R15)/(A$1)</f>
+        <v>91.666666666666671</v>
       </c>
       <c r="T15" s="15"/>
-      <c r="U15" s="15">
-        <v>60</v>
-      </c>
+      <c r="U15" s="15"/>
       <c r="V15" s="15"/>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
       <c r="Y15" s="18">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>SUM(T15:X15)</f>
+        <v>0</v>
       </c>
       <c r="Z15" s="15"/>
       <c r="AA15" s="6"/>
@@ -2377,66 +2449,70 @@
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z15:AD15)</f>
         <v>0</v>
       </c>
       <c r="AF15" s="15"/>
       <c r="AG15" s="24">
-        <f t="shared" si="4"/>
-        <v>41.333333333333336</v>
+        <f>K15*0.1+S15*0.2+Y15*0.2+AE15*0.2+AF15*0.3</f>
+        <v>31.666666666666671</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D16" s="12">
         <v>2</v>
       </c>
       <c r="E16" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="G16" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="18">
-        <f t="shared" si="0"/>
-        <v>83.333333333333329</v>
+        <f>100*SUM(D16:J16)/(2*A$1)</f>
+        <v>131.66666666666666</v>
       </c>
       <c r="L16" s="15">
         <v>100</v>
       </c>
       <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
         <v>60</v>
       </c>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
       <c r="O16" s="6">
-        <v>0</v>
-      </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="P16" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
       <c r="R16" s="6"/>
       <c r="S16" s="18">
-        <f t="shared" si="1"/>
-        <v>53.333333333333336</v>
+        <f>SUM(L16:R16)/(A$1)</f>
+        <v>76.666666666666671</v>
       </c>
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
@@ -2444,7 +2520,7 @@
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T16:X16)</f>
         <v>0</v>
       </c>
       <c r="Z16" s="15"/>
@@ -2453,27 +2529,27 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z16:AD16)</f>
         <v>0</v>
       </c>
       <c r="AF16" s="15"/>
       <c r="AG16" s="24">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>K16*0.1+S16*0.2+Y16*0.2+AE16*0.2+AF16*0.3</f>
+        <v>28.5</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D17" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="7">
         <v>2</v>
@@ -2482,21 +2558,21 @@
         <v>0</v>
       </c>
       <c r="G17" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I17" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="18">
-        <f t="shared" si="0"/>
-        <v>116.66666666666667</v>
+        <f>100*SUM(D17:J17)/(2*A$1)</f>
+        <v>100</v>
       </c>
       <c r="L17" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M17" s="6">
         <v>60</v>
@@ -2505,27 +2581,27 @@
         <v>0</v>
       </c>
       <c r="O17" s="6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="P17" s="6">
-        <v>95</v>
-      </c>
-      <c r="Q17" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>65</v>
+      </c>
       <c r="R17" s="6"/>
       <c r="S17" s="18">
-        <f t="shared" si="1"/>
-        <v>81.666666666666671</v>
+        <f>SUM(L17:R17)/(A$1)</f>
+        <v>75</v>
       </c>
       <c r="T17" s="15"/>
-      <c r="U17" s="15">
-        <v>60</v>
-      </c>
+      <c r="U17" s="15"/>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="18">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>SUM(T17:X17)</f>
+        <v>0</v>
       </c>
       <c r="Z17" s="15"/>
       <c r="AA17" s="6"/>
@@ -2533,13 +2609,13 @@
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z17:AD17)</f>
         <v>0</v>
       </c>
       <c r="AF17" s="15"/>
       <c r="AG17" s="24">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f>K17*0.1+S17*0.2+Y17*0.2+AE17*0.2+AF17*0.3</f>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2568,12 +2644,12 @@
         <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="18">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>100*SUM(D18:J18)/(2*A$1)</f>
+        <v>116.66666666666667</v>
       </c>
       <c r="L18" s="15">
         <v>0</v>
@@ -2587,12 +2663,16 @@
       <c r="O18" s="6">
         <v>60</v>
       </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>65</v>
+      </c>
       <c r="R18" s="6"/>
       <c r="S18" s="18">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f>SUM(L18:R18)/(A$1)</f>
+        <v>61.666666666666664</v>
       </c>
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
@@ -2600,7 +2680,7 @@
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T18:X18)</f>
         <v>0</v>
       </c>
       <c r="Z18" s="15"/>
@@ -2609,24 +2689,24 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z18:AD18)</f>
         <v>0</v>
       </c>
       <c r="AF18" s="15"/>
       <c r="AG18" s="24">
-        <f t="shared" si="4"/>
-        <v>18</v>
+        <f>K18*0.1+S18*0.2+Y18*0.2+AE18*0.2+AF18*0.3</f>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
@@ -2638,18 +2718,18 @@
         <v>0</v>
       </c>
       <c r="G19" s="7">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="18">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>100*SUM(D19:J19)/(2*A$1)</f>
+        <v>86.666666666666671</v>
       </c>
       <c r="L19" s="15">
         <v>0</v>
@@ -2663,12 +2743,16 @@
       <c r="O19" s="6">
         <v>50</v>
       </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
+      <c r="P19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>85</v>
+      </c>
       <c r="R19" s="6"/>
       <c r="S19" s="18">
-        <f t="shared" si="1"/>
-        <v>36.666666666666664</v>
+        <f>SUM(L19:R19)/(A$1)</f>
+        <v>65</v>
       </c>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
@@ -2676,7 +2760,7 @@
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
       <c r="Y19" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T19:X19)</f>
         <v>0</v>
       </c>
       <c r="Z19" s="15"/>
@@ -2685,24 +2769,24 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z19:AD19)</f>
         <v>0</v>
       </c>
       <c r="AF19" s="15"/>
       <c r="AG19" s="24">
-        <f t="shared" si="4"/>
-        <v>14.833333333333332</v>
+        <f>K19*0.1+S19*0.2+Y19*0.2+AE19*0.2+AF19*0.3</f>
+        <v>21.666666666666668</v>
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="D20" s="12">
         <v>0</v>
@@ -2714,18 +2798,18 @@
         <v>0</v>
       </c>
       <c r="G20" s="7">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="H20" s="7">
         <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="18">
-        <f t="shared" si="0"/>
-        <v>56.666666666666664</v>
+        <f>100*SUM(D20:J20)/(2*A$1)</f>
+        <v>91.666666666666671</v>
       </c>
       <c r="L20" s="15">
         <v>0</v>
@@ -2739,12 +2823,16 @@
       <c r="O20" s="6">
         <v>50</v>
       </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
+      <c r="P20" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>65</v>
+      </c>
       <c r="R20" s="6"/>
       <c r="S20" s="18">
-        <f t="shared" si="1"/>
-        <v>36.666666666666664</v>
+        <f>SUM(L20:R20)/(A$1)</f>
+        <v>58.333333333333336</v>
       </c>
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
@@ -2752,7 +2840,7 @@
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
       <c r="Y20" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T20:X20)</f>
         <v>0</v>
       </c>
       <c r="Z20" s="15"/>
@@ -2761,36 +2849,36 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z20:AD20)</f>
         <v>0</v>
       </c>
       <c r="AF20" s="15"/>
       <c r="AG20" s="24">
-        <f t="shared" si="4"/>
-        <v>13</v>
+        <f>K20*0.1+S20*0.2+Y20*0.2+AE20*0.2+AF20*0.3</f>
+        <v>20.833333333333336</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="D21" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E21" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
       </c>
       <c r="G21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="7">
         <v>0</v>
@@ -2800,36 +2888,42 @@
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="18">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>100*SUM(D21:J21)/(2*A$1)</f>
+        <v>33.333333333333336</v>
       </c>
       <c r="L21" s="15">
         <v>0</v>
       </c>
       <c r="M21" s="6">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="N21" s="6">
         <v>0</v>
       </c>
       <c r="O21" s="6">
-        <v>0</v>
-      </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>0</v>
+      </c>
       <c r="R21" s="6"/>
       <c r="S21" s="18">
-        <f t="shared" si="1"/>
-        <v>28.333333333333332</v>
+        <f>SUM(L21:R21)/(A$1)</f>
+        <v>20</v>
       </c>
       <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
+      <c r="U21" s="15">
+        <v>60</v>
+      </c>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(T21:X21)</f>
+        <v>60</v>
       </c>
       <c r="Z21" s="15"/>
       <c r="AA21" s="6"/>
@@ -2837,13 +2931,13 @@
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z21:AD21)</f>
         <v>0</v>
       </c>
       <c r="AF21" s="15"/>
       <c r="AG21" s="24">
-        <f t="shared" si="4"/>
-        <v>8.1666666666666679</v>
+        <f>K21*0.1+S21*0.2+Y21*0.2+AE21*0.2+AF21*0.3</f>
+        <v>19.333333333333336</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,7 +2968,7 @@
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D22:J22)/(2*A$1)</f>
         <v>66.666666666666671</v>
       </c>
       <c r="L22" s="15">
@@ -2892,11 +2986,13 @@
       <c r="P22" s="6">
         <v>10</v>
       </c>
-      <c r="Q22" s="6"/>
+      <c r="Q22" s="6">
+        <v>40</v>
+      </c>
       <c r="R22" s="6"/>
       <c r="S22" s="18">
-        <f t="shared" si="1"/>
-        <v>23.333333333333332</v>
+        <f>SUM(L22:R22)/(A$1)</f>
+        <v>36.666666666666664</v>
       </c>
       <c r="T22" s="15"/>
       <c r="U22" s="15"/>
@@ -2904,7 +3000,7 @@
       <c r="W22" s="15"/>
       <c r="X22" s="15"/>
       <c r="Y22" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T22:X22)</f>
         <v>0</v>
       </c>
       <c r="Z22" s="15"/>
@@ -2913,33 +3009,33 @@
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z22:AD22)</f>
         <v>0</v>
       </c>
       <c r="AF22" s="15"/>
       <c r="AG22" s="24">
-        <f t="shared" si="4"/>
-        <v>11.333333333333336</v>
+        <f>K22*0.1+S22*0.2+Y22*0.2+AE22*0.2+AF22*0.3</f>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D23" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" s="7">
         <v>0</v>
@@ -2952,27 +3048,31 @@
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="18">
-        <f t="shared" si="0"/>
-        <v>33.333333333333336</v>
+        <f>100*SUM(D23:J23)/(2*A$1)</f>
+        <v>25</v>
       </c>
       <c r="L23" s="15">
         <v>0</v>
       </c>
       <c r="M23" s="6">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="N23" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O23" s="6">
         <v>0</v>
       </c>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
+      <c r="P23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>0</v>
+      </c>
       <c r="R23" s="6"/>
       <c r="S23" s="18">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>SUM(L23:R23)/(A$1)</f>
+        <v>28.333333333333332</v>
       </c>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
@@ -2980,7 +3080,7 @@
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
       <c r="Y23" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T23:X23)</f>
         <v>0</v>
       </c>
       <c r="Z23" s="15"/>
@@ -2989,24 +3089,24 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
       <c r="AE23" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z23:AD23)</f>
         <v>0</v>
       </c>
       <c r="AF23" s="15"/>
       <c r="AG23" s="24">
-        <f t="shared" si="4"/>
-        <v>7.3333333333333339</v>
+        <f>K23*0.1+S23*0.2+Y23*0.2+AE23*0.2+AF23*0.3</f>
+        <v>8.1666666666666679</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="D24" s="12">
         <v>0</v>
@@ -3015,10 +3115,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
@@ -3028,7 +3128,7 @@
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D24:J24)/(2*A$1)</f>
         <v>33.333333333333336</v>
       </c>
       <c r="L24" s="15">
@@ -3038,28 +3138,30 @@
         <v>0</v>
       </c>
       <c r="N24" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O24" s="6">
-        <v>60</v>
-      </c>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
       <c r="R24" s="6"/>
       <c r="S24" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L24:R24)/(A$1)</f>
         <v>20</v>
       </c>
       <c r="T24" s="15"/>
-      <c r="U24" s="15">
-        <v>60</v>
-      </c>
+      <c r="U24" s="15"/>
       <c r="V24" s="15"/>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
       <c r="Y24" s="18">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>SUM(T24:X24)</f>
+        <v>0</v>
       </c>
       <c r="Z24" s="15"/>
       <c r="AA24" s="6"/>
@@ -3067,13 +3169,13 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
       <c r="AE24" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z24:AD24)</f>
         <v>0</v>
       </c>
       <c r="AF24" s="15"/>
       <c r="AG24" s="24">
-        <f t="shared" si="4"/>
-        <v>19.333333333333336</v>
+        <f>K24*0.1+S24*0.2+Y24*0.2+AE24*0.2+AF24*0.3</f>
+        <v>7.3333333333333339</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3106,7 +3208,7 @@
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D25:J25)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L25" s="15">
@@ -3121,11 +3223,15 @@
       <c r="O25" s="6">
         <v>0</v>
       </c>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
+      <c r="P25" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>0</v>
+      </c>
       <c r="R25" s="6"/>
       <c r="S25" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L25:R25)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T25" s="15"/>
@@ -3134,7 +3240,7 @@
       <c r="W25" s="15"/>
       <c r="X25" s="15"/>
       <c r="Y25" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T25:X25)</f>
         <v>0</v>
       </c>
       <c r="Z25" s="15"/>
@@ -3143,12 +3249,12 @@
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
       <c r="AE25" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z25:AD25)</f>
         <v>0</v>
       </c>
       <c r="AF25" s="15"/>
       <c r="AG25" s="24">
-        <f t="shared" si="4"/>
+        <f>K25*0.1+S25*0.2+Y25*0.2+AE25*0.2+AF25*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3182,7 +3288,7 @@
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D26:J26)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L26" s="15">
@@ -3197,11 +3303,15 @@
       <c r="O26" s="6">
         <v>0</v>
       </c>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
+      <c r="P26" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>0</v>
+      </c>
       <c r="R26" s="6"/>
       <c r="S26" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L26:R26)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T26" s="15"/>
@@ -3210,7 +3320,7 @@
       <c r="W26" s="15"/>
       <c r="X26" s="15"/>
       <c r="Y26" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T26:X26)</f>
         <v>0</v>
       </c>
       <c r="Z26" s="15"/>
@@ -3219,12 +3329,12 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z26:AD26)</f>
         <v>0</v>
       </c>
       <c r="AF26" s="15"/>
       <c r="AG26" s="24">
-        <f t="shared" si="4"/>
+        <f>K26*0.1+S26*0.2+Y26*0.2+AE26*0.2+AF26*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3258,7 +3368,7 @@
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D27:J27)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L27" s="15">
@@ -3273,11 +3383,15 @@
       <c r="O27" s="6">
         <v>0</v>
       </c>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
+      <c r="P27" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>0</v>
+      </c>
       <c r="R27" s="6"/>
       <c r="S27" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L27:R27)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T27" s="15"/>
@@ -3286,7 +3400,7 @@
       <c r="W27" s="15"/>
       <c r="X27" s="15"/>
       <c r="Y27" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T27:X27)</f>
         <v>0</v>
       </c>
       <c r="Z27" s="15"/>
@@ -3295,12 +3409,12 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
       <c r="AE27" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z27:AD27)</f>
         <v>0</v>
       </c>
       <c r="AF27" s="15"/>
       <c r="AG27" s="24">
-        <f t="shared" si="4"/>
+        <f>K27*0.1+S27*0.2+Y27*0.2+AE27*0.2+AF27*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3334,7 +3448,7 @@
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D28:J28)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L28" s="15">
@@ -3349,11 +3463,15 @@
       <c r="O28" s="6">
         <v>0</v>
       </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
+      <c r="P28" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>0</v>
+      </c>
       <c r="R28" s="6"/>
       <c r="S28" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L28:R28)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T28" s="15"/>
@@ -3362,7 +3480,7 @@
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T28:X28)</f>
         <v>0</v>
       </c>
       <c r="Z28" s="15"/>
@@ -3371,12 +3489,12 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
       <c r="AE28" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z28:AD28)</f>
         <v>0</v>
       </c>
       <c r="AF28" s="15"/>
       <c r="AG28" s="24">
-        <f t="shared" si="4"/>
+        <f>K28*0.1+S28*0.2+Y28*0.2+AE28*0.2+AF28*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3410,7 +3528,7 @@
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D29:J29)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L29" s="15">
@@ -3425,11 +3543,15 @@
       <c r="O29" s="6">
         <v>0</v>
       </c>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
+      <c r="P29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>0</v>
+      </c>
       <c r="R29" s="6"/>
       <c r="S29" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L29:R29)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T29" s="15"/>
@@ -3438,7 +3560,7 @@
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T29:X29)</f>
         <v>0</v>
       </c>
       <c r="Z29" s="15"/>
@@ -3447,12 +3569,12 @@
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
       <c r="AE29" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z29:AD29)</f>
         <v>0</v>
       </c>
       <c r="AF29" s="15"/>
       <c r="AG29" s="24">
-        <f t="shared" si="4"/>
+        <f>K29*0.1+S29*0.2+Y29*0.2+AE29*0.2+AF29*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3486,7 +3608,7 @@
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D30:J30)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L30" s="15">
@@ -3501,11 +3623,15 @@
       <c r="O30" s="6">
         <v>0</v>
       </c>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
+      <c r="P30" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>0</v>
+      </c>
       <c r="R30" s="6"/>
       <c r="S30" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L30:R30)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T30" s="15"/>
@@ -3514,7 +3640,7 @@
       <c r="W30" s="15"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T30:X30)</f>
         <v>0</v>
       </c>
       <c r="Z30" s="15"/>
@@ -3523,12 +3649,12 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
       <c r="AE30" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z30:AD30)</f>
         <v>0</v>
       </c>
       <c r="AF30" s="15"/>
       <c r="AG30" s="24">
-        <f t="shared" si="4"/>
+        <f>K30*0.1+S30*0.2+Y30*0.2+AE30*0.2+AF30*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3562,7 +3688,7 @@
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D31:J31)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L31" s="15">
@@ -3577,11 +3703,15 @@
       <c r="O31" s="6">
         <v>0</v>
       </c>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
+      <c r="P31" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>0</v>
+      </c>
       <c r="R31" s="6"/>
       <c r="S31" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L31:R31)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T31" s="15"/>
@@ -3590,7 +3720,7 @@
       <c r="W31" s="15"/>
       <c r="X31" s="15"/>
       <c r="Y31" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T31:X31)</f>
         <v>0</v>
       </c>
       <c r="Z31" s="15"/>
@@ -3599,12 +3729,12 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
       <c r="AE31" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z31:AD31)</f>
         <v>0</v>
       </c>
       <c r="AF31" s="15"/>
       <c r="AG31" s="24">
-        <f t="shared" si="4"/>
+        <f>K31*0.1+S31*0.2+Y31*0.2+AE31*0.2+AF31*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3638,7 +3768,7 @@
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D32:J32)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L32" s="15">
@@ -3653,11 +3783,15 @@
       <c r="O32" s="6">
         <v>0</v>
       </c>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
+      <c r="P32" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>0</v>
+      </c>
       <c r="R32" s="6"/>
       <c r="S32" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L32:R32)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T32" s="15"/>
@@ -3666,7 +3800,7 @@
       <c r="W32" s="15"/>
       <c r="X32" s="15"/>
       <c r="Y32" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(T32:X32)</f>
         <v>0</v>
       </c>
       <c r="Z32" s="15"/>
@@ -3675,12 +3809,12 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
       <c r="AE32" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z32:AD32)</f>
         <v>0</v>
       </c>
       <c r="AF32" s="15"/>
       <c r="AG32" s="24">
-        <f t="shared" si="4"/>
+        <f>K32*0.1+S32*0.2+Y32*0.2+AE32*0.2+AF32*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -3714,7 +3848,7 @@
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="18">
-        <f t="shared" si="0"/>
+        <f>100*SUM(D33:J33)/(2*A$1)</f>
         <v>0</v>
       </c>
       <c r="L33" s="15">
@@ -3729,11 +3863,15 @@
       <c r="O33" s="17">
         <v>0</v>
       </c>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
+      <c r="P33" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>0</v>
+      </c>
       <c r="R33" s="17"/>
       <c r="S33" s="18">
-        <f t="shared" si="1"/>
+        <f>SUM(L33:R33)/(A$1)</f>
         <v>0</v>
       </c>
       <c r="T33" s="15"/>
@@ -3742,7 +3880,7 @@
       <c r="W33" s="15"/>
       <c r="X33" s="15"/>
       <c r="Y33" s="20">
-        <f t="shared" si="2"/>
+        <f>SUM(T33:X33)</f>
         <v>0</v>
       </c>
       <c r="Z33" s="16"/>
@@ -3751,12 +3889,12 @@
       <c r="AC33" s="17"/>
       <c r="AD33" s="17"/>
       <c r="AE33" s="18">
-        <f t="shared" si="3"/>
+        <f>SUM(Z33:AD33)</f>
         <v>0</v>
       </c>
       <c r="AF33" s="16"/>
       <c r="AG33" s="28">
-        <f t="shared" si="4"/>
+        <f>K33*0.1+S33*0.2+Y33*0.2+AE33*0.2+AF33*0.3</f>
         <v>0</v>
       </c>
     </row>
@@ -5049,14 +5187,14 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J33">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5131,35 +5269,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R33">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:X33">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>

</xml_diff>

<commit_message>
Ileri java odev 1-2 not guncelleme
</commit_message>
<xml_diff>
--- a/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
+++ b/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
@@ -782,7 +782,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -818,6 +818,74 @@
         <patternFill>
           <fgColor auto="1"/>
           <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1212,7 +1280,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ15" sqref="AJ15"/>
+      <selection pane="bottomLeft" activeCell="AM14" sqref="AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1309,7 @@
   <sheetData>
     <row r="1" spans="1:34" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="34"/>
@@ -1420,7 +1488,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="18">
         <f>100*SUM(D3:J3)/(2*A$1)</f>
-        <v>161.66666666666666</v>
+        <v>96.999999999999986</v>
       </c>
       <c r="L3" s="15">
         <v>90</v>
@@ -1443,20 +1511,20 @@
       <c r="R3" s="6"/>
       <c r="S3" s="18">
         <f>SUM(L3:R3)/(A$1)</f>
-        <v>193.33333333333334</v>
+        <v>116</v>
       </c>
       <c r="T3" s="15">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="U3" s="15">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="18">
         <f>SUM(T3:X3)</f>
-        <v>120</v>
+        <v>210</v>
       </c>
       <c r="Z3" s="15"/>
       <c r="AA3" s="6"/>
@@ -1470,7 +1538,7 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="24">
         <f>K3*0.1+S3*0.2+Y3*0.2+AE3*0.2+AF3*0.3</f>
-        <v>78.833333333333343</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>103</v>
@@ -1507,7 +1575,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="18">
         <f>100*SUM(D4:J4)/(2*A$1)</f>
-        <v>166.66666666666666</v>
+        <v>100</v>
       </c>
       <c r="L4" s="15">
         <v>0</v>
@@ -1530,20 +1598,20 @@
       <c r="R4" s="6"/>
       <c r="S4" s="18">
         <f>SUM(L4:R4)/(A$1)</f>
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="T4" s="15">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="U4" s="15">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="18">
         <f>SUM(T4:X4)</f>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="Z4" s="15"/>
       <c r="AA4" s="6"/>
@@ -1557,21 +1625,21 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="24">
         <f>K4*0.1+S4*0.2+Y4*0.2+AE4*0.2+AF4*0.3</f>
-        <v>73.666666666666671</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D5" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
         <v>2</v>
@@ -1583,51 +1651,51 @@
         <v>2</v>
       </c>
       <c r="H5" s="7">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="I5" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="18">
         <f>100*SUM(D5:J5)/(2*A$1)</f>
-        <v>183.33333333333334</v>
+        <v>96.999999999999986</v>
       </c>
       <c r="L5" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M5" s="6">
         <v>100</v>
       </c>
       <c r="N5" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O5" s="6">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="P5" s="6">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="Q5" s="6">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="18">
         <f>SUM(L5:R5)/(A$1)</f>
-        <v>153.33333333333334</v>
+        <v>95</v>
       </c>
       <c r="T5" s="15">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="U5" s="15">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
       <c r="Y5" s="18">
         <f>SUM(T5:X5)</f>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="Z5" s="15"/>
       <c r="AA5" s="6"/>
@@ -1641,21 +1709,21 @@
       <c r="AF5" s="15"/>
       <c r="AG5" s="24">
         <f>K5*0.1+S5*0.2+Y5*0.2+AE5*0.2+AF5*0.3</f>
-        <v>73</v>
+        <v>67.7</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="7">
         <v>2</v>
@@ -1667,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="7">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="I6" s="7">
         <v>2</v>
@@ -1675,19 +1743,19 @@
       <c r="J6" s="7"/>
       <c r="K6" s="18">
         <f>100*SUM(D6:J6)/(2*A$1)</f>
-        <v>161.66666666666666</v>
+        <v>120</v>
       </c>
       <c r="L6" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M6" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="N6" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O6" s="6">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="P6" s="6">
         <v>90</v>
@@ -1698,20 +1766,20 @@
       <c r="R6" s="6"/>
       <c r="S6" s="18">
         <f>SUM(L6:R6)/(A$1)</f>
-        <v>158.33333333333334</v>
+        <v>92</v>
       </c>
       <c r="T6" s="15">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="U6" s="15">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="V6" s="15"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
       <c r="Y6" s="18">
         <f>SUM(T6:X6)</f>
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="Z6" s="15"/>
       <c r="AA6" s="6"/>
@@ -1725,21 +1793,21 @@
       <c r="AF6" s="15"/>
       <c r="AG6" s="24">
         <f>K6*0.1+S6*0.2+Y6*0.2+AE6*0.2+AF6*0.3</f>
-        <v>71.833333333333343</v>
+        <v>62.400000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -1751,7 +1819,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="I7" s="7">
         <v>2</v>
@@ -1759,43 +1827,43 @@
       <c r="J7" s="7"/>
       <c r="K7" s="18">
         <f>100*SUM(D7:J7)/(2*A$1)</f>
-        <v>166.66666666666666</v>
+        <v>118</v>
       </c>
       <c r="L7" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M7" s="6">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N7" s="6">
+        <v>60</v>
+      </c>
+      <c r="O7" s="6">
+        <v>60</v>
+      </c>
+      <c r="P7" s="6">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="6">
         <v>80</v>
-      </c>
-      <c r="O7" s="6">
-        <v>90</v>
-      </c>
-      <c r="P7" s="6">
-        <v>95</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>95</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="18">
         <f>SUM(L7:R7)/(A$1)</f>
-        <v>153.33333333333334</v>
+        <v>88</v>
       </c>
       <c r="T7" s="15">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="U7" s="15">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="18">
         <f>SUM(T7:X7)</f>
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="Z7" s="15"/>
       <c r="AA7" s="6"/>
@@ -1809,18 +1877,18 @@
       <c r="AF7" s="15"/>
       <c r="AG7" s="24">
         <f>K7*0.1+S7*0.2+Y7*0.2+AE7*0.2+AF7*0.3</f>
-        <v>71.333333333333343</v>
+        <v>61.400000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D8" s="12">
         <v>2</v>
@@ -1838,46 +1906,48 @@
         <v>2</v>
       </c>
       <c r="I8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="18">
         <f>100*SUM(D8:J8)/(2*A$1)</f>
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="L8" s="15">
         <v>100</v>
       </c>
       <c r="M8" s="6">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="N8" s="6">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="O8" s="6">
         <v>60</v>
       </c>
       <c r="P8" s="6">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="Q8" s="6">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="18">
         <f>SUM(L8:R8)/(A$1)</f>
-        <v>153.33333333333334</v>
-      </c>
-      <c r="T8" s="15"/>
+        <v>92</v>
+      </c>
+      <c r="T8" s="15">
+        <v>70</v>
+      </c>
       <c r="U8" s="15">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="V8" s="15"/>
       <c r="W8" s="15"/>
       <c r="X8" s="15"/>
       <c r="Y8" s="18">
         <f>SUM(T8:X8)</f>
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="Z8" s="15"/>
       <c r="AA8" s="6"/>
@@ -1891,21 +1961,21 @@
       <c r="AF8" s="15"/>
       <c r="AG8" s="24">
         <f>K8*0.1+S8*0.2+Y8*0.2+AE8*0.2+AF8*0.3</f>
-        <v>62.666666666666671</v>
+        <v>60.400000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D9" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
@@ -1914,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="H9" s="7">
         <v>2</v>
@@ -1925,22 +1995,22 @@
       <c r="J9" s="7"/>
       <c r="K9" s="18">
         <f>100*SUM(D9:J9)/(2*A$1)</f>
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="L9" s="15">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
         <v>100</v>
-      </c>
-      <c r="M9" s="6">
-        <v>80</v>
       </c>
       <c r="N9" s="6">
         <v>80</v>
       </c>
       <c r="O9" s="6">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="P9" s="6">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q9" s="6">
         <v>95</v>
@@ -1948,16 +2018,20 @@
       <c r="R9" s="6"/>
       <c r="S9" s="18">
         <f>SUM(L9:R9)/(A$1)</f>
-        <v>171.66666666666666</v>
-      </c>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
+        <v>92</v>
+      </c>
+      <c r="T9" s="15">
+        <v>75</v>
+      </c>
+      <c r="U9" s="15">
+        <v>80</v>
+      </c>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="18">
         <f>SUM(T9:X9)</f>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="Z9" s="15"/>
       <c r="AA9" s="6"/>
@@ -1971,7 +2045,7 @@
       <c r="AF9" s="15"/>
       <c r="AG9" s="24">
         <f>K9*0.1+S9*0.2+Y9*0.2+AE9*0.2+AF9*0.3</f>
-        <v>53.333333333333336</v>
+        <v>59.400000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2005,7 +2079,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="18">
         <f>100*SUM(D10:J10)/(2*A$1)</f>
-        <v>133.33333333333334</v>
+        <v>80</v>
       </c>
       <c r="L10" s="15">
         <v>0</v>
@@ -2028,18 +2102,20 @@
       <c r="R10" s="6"/>
       <c r="S10" s="18">
         <f>SUM(L10:R10)/(A$1)</f>
-        <v>120</v>
-      </c>
-      <c r="T10" s="15"/>
+        <v>72</v>
+      </c>
+      <c r="T10" s="15">
+        <v>95</v>
+      </c>
       <c r="U10" s="15">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="V10" s="15"/>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="18">
         <f>SUM(T10:X10)</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="Z10" s="15"/>
       <c r="AA10" s="6"/>
@@ -2053,33 +2129,33 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="24">
         <f>K10*0.1+S10*0.2+Y10*0.2+AE10*0.2+AF10*0.3</f>
-        <v>49.333333333333336</v>
+        <v>58.4</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D11" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
       </c>
       <c r="F11" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="7">
         <v>2</v>
       </c>
       <c r="H11" s="7">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="I11" s="7">
         <v>2</v>
@@ -2087,39 +2163,43 @@
       <c r="J11" s="7"/>
       <c r="K11" s="18">
         <f>100*SUM(D11:J11)/(2*A$1)</f>
-        <v>196.66666666666666</v>
+        <v>80</v>
       </c>
       <c r="L11" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M11" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="N11" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O11" s="6">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="P11" s="6">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="Q11" s="6">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="18">
         <f>SUM(L11:R11)/(A$1)</f>
-        <v>146.66666666666666</v>
-      </c>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
+        <v>68</v>
+      </c>
+      <c r="T11" s="15">
+        <v>75</v>
+      </c>
+      <c r="U11" s="15">
+        <v>80</v>
+      </c>
       <c r="V11" s="15"/>
       <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="18">
         <f>SUM(T11:X11)</f>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="Z11" s="15"/>
       <c r="AA11" s="6"/>
@@ -2133,24 +2213,24 @@
       <c r="AF11" s="15"/>
       <c r="AG11" s="24">
         <f>K11*0.1+S11*0.2+Y11*0.2+AE11*0.2+AF11*0.3</f>
-        <v>49</v>
+        <v>52.6</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D12" s="12">
         <v>0</v>
       </c>
       <c r="E12" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
@@ -2159,49 +2239,51 @@
         <v>2</v>
       </c>
       <c r="H12" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="18">
         <f>100*SUM(D12:J12)/(2*A$1)</f>
-        <v>133.33333333333334</v>
+        <v>20</v>
       </c>
       <c r="L12" s="15">
         <v>0</v>
       </c>
       <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
         <v>60</v>
       </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="6">
-        <v>90</v>
-      </c>
       <c r="P12" s="6">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="6">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="18">
         <f>SUM(L12:R12)/(A$1)</f>
-        <v>113.33333333333333</v>
-      </c>
-      <c r="T12" s="15"/>
+        <v>12</v>
+      </c>
+      <c r="T12" s="15">
+        <v>90</v>
+      </c>
       <c r="U12" s="15">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="V12" s="15"/>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="18">
         <f>SUM(T12:X12)</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="Z12" s="15"/>
       <c r="AA12" s="6"/>
@@ -2215,21 +2297,21 @@
       <c r="AF12" s="15"/>
       <c r="AG12" s="24">
         <f>K12*0.1+S12*0.2+Y12*0.2+AE12*0.2+AF12*0.3</f>
-        <v>48</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -2238,10 +2320,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="7">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="H13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="7">
         <v>2</v>
@@ -2249,30 +2331,30 @@
       <c r="J13" s="7"/>
       <c r="K13" s="18">
         <f>100*SUM(D13:J13)/(2*A$1)</f>
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="L13" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M13" s="6">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="N13" s="6">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="O13" s="6">
         <v>60</v>
       </c>
       <c r="P13" s="6">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="6">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="R13" s="6"/>
       <c r="S13" s="18">
         <f>SUM(L13:R13)/(A$1)</f>
-        <v>93.333333333333329</v>
+        <v>103</v>
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
@@ -2295,18 +2377,18 @@
       <c r="AF13" s="15"/>
       <c r="AG13" s="24">
         <f>K13*0.1+S13*0.2+Y13*0.2+AE13*0.2+AF13*0.3</f>
-        <v>33.666666666666671</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
@@ -2329,7 +2411,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="18">
         <f>100*SUM(D14:J14)/(2*A$1)</f>
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="L14" s="15">
         <v>0</v>
@@ -2344,15 +2426,15 @@
         <v>60</v>
       </c>
       <c r="P14" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q14" s="6">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="18">
         <f>SUM(L14:R14)/(A$1)</f>
-        <v>88.333333333333329</v>
+        <v>56</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
@@ -2375,18 +2457,18 @@
       <c r="AF14" s="15"/>
       <c r="AG14" s="24">
         <f>K14*0.1+S14*0.2+Y14*0.2+AE14*0.2+AF14*0.3</f>
-        <v>32.666666666666671</v>
+        <v>20.200000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -2401,7 +2483,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="7">
         <v>2</v>
@@ -2409,30 +2491,30 @@
       <c r="J15" s="7"/>
       <c r="K15" s="18">
         <f>100*SUM(D15:J15)/(2*A$1)</f>
-        <v>133.33333333333334</v>
+        <v>90</v>
       </c>
       <c r="L15" s="15">
         <v>0</v>
       </c>
       <c r="M15" s="6">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="N15" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="O15" s="6">
         <v>60</v>
       </c>
       <c r="P15" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q15" s="6">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="18">
         <f>SUM(L15:R15)/(A$1)</f>
-        <v>91.666666666666671</v>
+        <v>53</v>
       </c>
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
@@ -2455,64 +2537,64 @@
       <c r="AF15" s="15"/>
       <c r="AG15" s="24">
         <f>K15*0.1+S15*0.2+Y15*0.2+AE15*0.2+AF15*0.3</f>
-        <v>31.666666666666671</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D16" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="7">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="G16" s="7">
         <v>2</v>
       </c>
       <c r="H16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="18">
         <f>100*SUM(D16:J16)/(2*A$1)</f>
-        <v>131.66666666666666</v>
+        <v>80</v>
       </c>
       <c r="L16" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N16" s="6">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="O16" s="6">
         <v>60</v>
       </c>
       <c r="P16" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="6">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="18">
         <f>SUM(L16:R16)/(A$1)</f>
-        <v>76.666666666666671</v>
+        <v>55</v>
       </c>
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
@@ -2535,64 +2617,64 @@
       <c r="AF16" s="15"/>
       <c r="AG16" s="24">
         <f>K16*0.1+S16*0.2+Y16*0.2+AE16*0.2+AF16*0.3</f>
-        <v>28.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D17" s="12">
         <v>2</v>
       </c>
       <c r="E17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="G17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="18">
         <f>100*SUM(D17:J17)/(2*A$1)</f>
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="L17" s="15">
         <v>100</v>
       </c>
       <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
         <v>60</v>
       </c>
-      <c r="N17" s="6">
-        <v>0</v>
-      </c>
       <c r="O17" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P17" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="6">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="18">
         <f>SUM(L17:R17)/(A$1)</f>
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
@@ -2615,30 +2697,30 @@
       <c r="AF17" s="15"/>
       <c r="AG17" s="24">
         <f>K17*0.1+S17*0.2+Y17*0.2+AE17*0.2+AF17*0.3</f>
-        <v>25</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D18" s="12">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F18" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -2649,19 +2731,19 @@
       <c r="J18" s="7"/>
       <c r="K18" s="18">
         <f>100*SUM(D18:J18)/(2*A$1)</f>
-        <v>116.66666666666667</v>
+        <v>60</v>
       </c>
       <c r="L18" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N18" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O18" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="P18" s="6">
         <v>0</v>
@@ -2672,7 +2754,7 @@
       <c r="R18" s="6"/>
       <c r="S18" s="18">
         <f>SUM(L18:R18)/(A$1)</f>
-        <v>61.666666666666664</v>
+        <v>45</v>
       </c>
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
@@ -2695,64 +2777,64 @@
       <c r="AF18" s="15"/>
       <c r="AG18" s="24">
         <f>K18*0.1+S18*0.2+Y18*0.2+AE18*0.2+AF18*0.3</f>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D19" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="7">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="18">
         <f>100*SUM(D19:J19)/(2*A$1)</f>
-        <v>86.666666666666671</v>
+        <v>70</v>
       </c>
       <c r="L19" s="15">
         <v>0</v>
       </c>
       <c r="M19" s="6">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6">
         <v>60</v>
       </c>
-      <c r="N19" s="6">
-        <v>0</v>
-      </c>
       <c r="O19" s="6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="P19" s="6">
         <v>0</v>
       </c>
       <c r="Q19" s="6">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="R19" s="6"/>
       <c r="S19" s="18">
         <f>SUM(L19:R19)/(A$1)</f>
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
@@ -2775,18 +2857,18 @@
       <c r="AF19" s="15"/>
       <c r="AG19" s="24">
         <f>K19*0.1+S19*0.2+Y19*0.2+AE19*0.2+AF19*0.3</f>
-        <v>21.666666666666668</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="20" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D20" s="12">
         <v>0</v>
@@ -2798,18 +2880,18 @@
         <v>0</v>
       </c>
       <c r="G20" s="7">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="H20" s="7">
         <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="18">
         <f>100*SUM(D20:J20)/(2*A$1)</f>
-        <v>91.666666666666671</v>
+        <v>52</v>
       </c>
       <c r="L20" s="15">
         <v>0</v>
@@ -2827,12 +2909,12 @@
         <v>0</v>
       </c>
       <c r="Q20" s="6">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="R20" s="6"/>
       <c r="S20" s="18">
         <f>SUM(L20:R20)/(A$1)</f>
-        <v>58.333333333333336</v>
+        <v>39</v>
       </c>
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
@@ -2855,75 +2937,73 @@
       <c r="AF20" s="15"/>
       <c r="AG20" s="24">
         <f>K20*0.1+S20*0.2+Y20*0.2+AE20*0.2+AF20*0.3</f>
-        <v>20.833333333333336</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="D21" s="12">
         <v>0</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
       </c>
       <c r="G21" s="7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H21" s="7">
         <v>0</v>
       </c>
       <c r="I21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="18">
         <f>100*SUM(D21:J21)/(2*A$1)</f>
-        <v>33.333333333333336</v>
+        <v>55</v>
       </c>
       <c r="L21" s="15">
         <v>0</v>
       </c>
       <c r="M21" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N21" s="6">
         <v>0</v>
       </c>
       <c r="O21" s="6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="P21" s="6">
         <v>0</v>
       </c>
       <c r="Q21" s="6">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="18">
         <f>SUM(L21:R21)/(A$1)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="T21" s="15"/>
-      <c r="U21" s="15">
-        <v>60</v>
-      </c>
+      <c r="U21" s="15"/>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="18">
         <f>SUM(T21:X21)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="15"/>
       <c r="AA21" s="6"/>
@@ -2937,16 +3017,18 @@
       <c r="AF21" s="15"/>
       <c r="AG21" s="24">
         <f>K21*0.1+S21*0.2+Y21*0.2+AE21*0.2+AF21*0.3</f>
-        <v>19.333333333333336</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" s="3" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
       <c r="D22" s="12">
         <v>0</v>
@@ -2955,21 +3037,21 @@
         <v>0</v>
       </c>
       <c r="F22" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="7">
         <v>0</v>
       </c>
       <c r="H22" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="18">
         <f>100*SUM(D22:J22)/(2*A$1)</f>
-        <v>66.666666666666671</v>
+        <v>0</v>
       </c>
       <c r="L22" s="15">
         <v>0</v>
@@ -2978,30 +3060,34 @@
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O22" s="6">
         <v>0</v>
       </c>
       <c r="P22" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="6">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="18">
         <f>SUM(L22:R22)/(A$1)</f>
-        <v>36.666666666666664</v>
-      </c>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="15">
+        <v>30</v>
+      </c>
+      <c r="U22" s="15">
+        <v>30</v>
+      </c>
       <c r="V22" s="15"/>
       <c r="W22" s="15"/>
       <c r="X22" s="15"/>
       <c r="Y22" s="18">
         <f>SUM(T22:X22)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Z22" s="15"/>
       <c r="AA22" s="6"/>
@@ -3015,64 +3101,62 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="24">
         <f>K22*0.1+S22*0.2+Y22*0.2+AE22*0.2+AF22*0.3</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>31</v>
-      </c>
+      <c r="A23" s="23"/>
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="D23" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
         <v>1</v>
       </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="7">
-        <v>0</v>
-      </c>
-      <c r="H23" s="7">
-        <v>0</v>
-      </c>
       <c r="I23" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="18">
         <f>100*SUM(D23:J23)/(2*A$1)</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L23" s="15">
         <v>0</v>
       </c>
       <c r="M23" s="6">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="N23" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O23" s="6">
         <v>0</v>
       </c>
       <c r="P23" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q23" s="6">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R23" s="6"/>
       <c r="S23" s="18">
         <f>SUM(L23:R23)/(A$1)</f>
-        <v>28.333333333333332</v>
+        <v>22</v>
       </c>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
@@ -3095,27 +3179,27 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="24">
         <f>K23*0.1+S23*0.2+Y23*0.2+AE23*0.2+AF23*0.3</f>
-        <v>8.1666666666666679</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D24" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="7">
         <v>0</v>
@@ -3129,16 +3213,16 @@
       <c r="J24" s="7"/>
       <c r="K24" s="18">
         <f>100*SUM(D24:J24)/(2*A$1)</f>
-        <v>33.333333333333336</v>
+        <v>15</v>
       </c>
       <c r="L24" s="15">
         <v>0</v>
       </c>
       <c r="M24" s="6">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="N24" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O24" s="6">
         <v>0</v>
@@ -3152,7 +3236,7 @@
       <c r="R24" s="6"/>
       <c r="S24" s="18">
         <f>SUM(L24:R24)/(A$1)</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="15"/>
@@ -3175,18 +3259,18 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="24">
         <f>K24*0.1+S24*0.2+Y24*0.2+AE24*0.2+AF24*0.3</f>
-        <v>7.3333333333333339</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D25" s="12">
         <v>0</v>
@@ -3195,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="7">
         <v>0</v>
@@ -3209,7 +3293,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="18">
         <f>100*SUM(D25:J25)/(2*A$1)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L25" s="15">
         <v>0</v>
@@ -3218,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O25" s="6">
         <v>0</v>
@@ -3232,7 +3316,7 @@
       <c r="R25" s="6"/>
       <c r="S25" s="18">
         <f>SUM(L25:R25)/(A$1)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
@@ -3255,18 +3339,18 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="24">
         <f>K25*0.1+S25*0.2+Y25*0.2+AE25*0.2+AF25*0.3</f>
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D26" s="12">
         <v>0</v>
@@ -3340,13 +3424,13 @@
     </row>
     <row r="27" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D27" s="12">
         <v>0</v>
@@ -3420,13 +3504,13 @@
     </row>
     <row r="28" spans="1:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D28" s="12">
         <v>0</v>
@@ -5178,7 +5262,7 @@
     </row>
   </sheetData>
   <sortState ref="A3:AH33">
-    <sortCondition descending="1" ref="AG2"/>
+    <sortCondition descending="1" ref="AG3"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="T1:Y1"/>
@@ -5187,14 +5271,14 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J33">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5269,37 +5353,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R33">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:X33">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="between">
       <formula>80</formula>
-      <formula>100</formula>
+      <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ileri java ders icerik
</commit_message>
<xml_diff>
--- a/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
+++ b/AdvancedJava_2017Autumn/_docs/NotlarIleriJavaGuz2017.xlsx
@@ -766,7 +766,83 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1264,7 +1340,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL24" sqref="AL24"/>
+      <selection pane="bottomLeft" activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2340,8 +2416,12 @@
         <f>SUM(L13:R13)/(A$1)</f>
         <v>103</v>
       </c>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
+      <c r="T13" s="15">
+        <v>0</v>
+      </c>
+      <c r="U13" s="15">
+        <v>0</v>
+      </c>
       <c r="V13" s="15"/>
       <c r="W13" s="15"/>
       <c r="X13" s="15"/>
@@ -2420,8 +2500,12 @@
         <f>SUM(L14:R14)/(A$1)</f>
         <v>56</v>
       </c>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
+      <c r="T14" s="15">
+        <v>0</v>
+      </c>
+      <c r="U14" s="15">
+        <v>0</v>
+      </c>
       <c r="V14" s="15"/>
       <c r="W14" s="15"/>
       <c r="X14" s="15"/>
@@ -2500,8 +2584,12 @@
         <f>SUM(L15:R15)/(A$1)</f>
         <v>53</v>
       </c>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
+      <c r="T15" s="15">
+        <v>0</v>
+      </c>
+      <c r="U15" s="15">
+        <v>0</v>
+      </c>
       <c r="V15" s="15"/>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
@@ -2580,8 +2668,12 @@
         <f>SUM(L16:R16)/(A$1)</f>
         <v>55</v>
       </c>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
+      <c r="T16" s="15">
+        <v>0</v>
+      </c>
+      <c r="U16" s="15">
+        <v>0</v>
+      </c>
       <c r="V16" s="15"/>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
@@ -2660,8 +2752,12 @@
         <f>SUM(L17:R17)/(A$1)</f>
         <v>46</v>
       </c>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
+      <c r="T17" s="15">
+        <v>0</v>
+      </c>
+      <c r="U17" s="15">
+        <v>0</v>
+      </c>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
@@ -2740,8 +2836,12 @@
         <f>SUM(L18:R18)/(A$1)</f>
         <v>45</v>
       </c>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
+      <c r="T18" s="15">
+        <v>0</v>
+      </c>
+      <c r="U18" s="15">
+        <v>0</v>
+      </c>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
@@ -2820,8 +2920,12 @@
         <f>SUM(L19:R19)/(A$1)</f>
         <v>37</v>
       </c>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
+      <c r="T19" s="15">
+        <v>0</v>
+      </c>
+      <c r="U19" s="15">
+        <v>0</v>
+      </c>
       <c r="V19" s="15"/>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
@@ -2900,8 +3004,12 @@
         <f>SUM(L20:R20)/(A$1)</f>
         <v>39</v>
       </c>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
+      <c r="T20" s="15">
+        <v>0</v>
+      </c>
+      <c r="U20" s="15">
+        <v>0</v>
+      </c>
       <c r="V20" s="15"/>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
@@ -2980,8 +3088,12 @@
         <f>SUM(L21:R21)/(A$1)</f>
         <v>35</v>
       </c>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
+      <c r="T21" s="15">
+        <v>0</v>
+      </c>
+      <c r="U21" s="15">
+        <v>0</v>
+      </c>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
@@ -3142,8 +3254,12 @@
         <f>SUM(L23:R23)/(A$1)</f>
         <v>22</v>
       </c>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
+      <c r="T23" s="15">
+        <v>0</v>
+      </c>
+      <c r="U23" s="15">
+        <v>0</v>
+      </c>
       <c r="V23" s="15"/>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
@@ -3222,8 +3338,12 @@
         <f>SUM(L24:R24)/(A$1)</f>
         <v>17</v>
       </c>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
+      <c r="T24" s="15">
+        <v>0</v>
+      </c>
+      <c r="U24" s="15">
+        <v>0</v>
+      </c>
       <c r="V24" s="15"/>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
@@ -3302,8 +3422,12 @@
         <f>SUM(L25:R25)/(A$1)</f>
         <v>12</v>
       </c>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
+      <c r="T25" s="15">
+        <v>0</v>
+      </c>
+      <c r="U25" s="15">
+        <v>0</v>
+      </c>
       <c r="V25" s="15"/>
       <c r="W25" s="15"/>
       <c r="X25" s="15"/>
@@ -3382,8 +3506,12 @@
         <f>SUM(L26:R26)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
+      <c r="T26" s="15">
+        <v>0</v>
+      </c>
+      <c r="U26" s="15">
+        <v>0</v>
+      </c>
       <c r="V26" s="15"/>
       <c r="W26" s="15"/>
       <c r="X26" s="15"/>
@@ -3462,8 +3590,12 @@
         <f>SUM(L27:R27)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
+      <c r="T27" s="15">
+        <v>0</v>
+      </c>
+      <c r="U27" s="15">
+        <v>0</v>
+      </c>
       <c r="V27" s="15"/>
       <c r="W27" s="15"/>
       <c r="X27" s="15"/>
@@ -3542,8 +3674,12 @@
         <f>SUM(L28:R28)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
+      <c r="T28" s="15">
+        <v>0</v>
+      </c>
+      <c r="U28" s="15">
+        <v>0</v>
+      </c>
       <c r="V28" s="15"/>
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
@@ -3622,8 +3758,12 @@
         <f>SUM(L29:R29)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
+      <c r="T29" s="15">
+        <v>0</v>
+      </c>
+      <c r="U29" s="15">
+        <v>0</v>
+      </c>
       <c r="V29" s="15"/>
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
@@ -3702,8 +3842,12 @@
         <f>SUM(L30:R30)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
+      <c r="T30" s="15">
+        <v>0</v>
+      </c>
+      <c r="U30" s="15">
+        <v>0</v>
+      </c>
       <c r="V30" s="15"/>
       <c r="W30" s="15"/>
       <c r="X30" s="15"/>
@@ -3782,8 +3926,12 @@
         <f>SUM(L31:R31)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
+      <c r="T31" s="15">
+        <v>0</v>
+      </c>
+      <c r="U31" s="15">
+        <v>0</v>
+      </c>
       <c r="V31" s="15"/>
       <c r="W31" s="15"/>
       <c r="X31" s="15"/>
@@ -3862,8 +4010,12 @@
         <f>SUM(L32:R32)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
+      <c r="T32" s="15">
+        <v>0</v>
+      </c>
+      <c r="U32" s="15">
+        <v>0</v>
+      </c>
       <c r="V32" s="15"/>
       <c r="W32" s="15"/>
       <c r="X32" s="15"/>
@@ -3942,8 +4094,12 @@
         <f>SUM(L33:R33)/(A$1)</f>
         <v>0</v>
       </c>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
+      <c r="T33" s="15">
+        <v>0</v>
+      </c>
+      <c r="U33" s="15">
+        <v>0</v>
+      </c>
       <c r="V33" s="15"/>
       <c r="W33" s="15"/>
       <c r="X33" s="15"/>
@@ -5255,14 +5411,14 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J33">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="14" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5337,35 +5493,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R33">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:X33">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="between">
       <formula>80</formula>
       <formula>200</formula>
     </cfRule>

</xml_diff>